<commit_message>
Bug fix in translation lists for optional parameters
</commit_message>
<xml_diff>
--- a/libs/ReferenceData/Maple.xlsx
+++ b/libs/ReferenceData/Maple.xlsx
@@ -2008,9 +2008,6 @@
     <t>\Lameb{n}{\nu}@{k^2}</t>
   </si>
   <si>
-    <t>LegendreP($1, $0, $2)</t>
-  </si>
-  <si>
     <t>https://www.maplesoft.com/support/help/maple/view.aspx?path=LegendreP</t>
   </si>
   <si>
@@ -3415,31 +3412,34 @@
     <t>\FerrersP{\nu}@{z}</t>
   </si>
   <si>
-    <t>X1X\FerrersP[\mu]{\nu}@{z}</t>
-  </si>
-  <si>
     <t>\FerrersQ{\nu}@{z}</t>
   </si>
   <si>
-    <t>X1X\FerrersQ[\mu]{\nu}@{z}</t>
-  </si>
-  <si>
     <t>\LegendreBlackQ{\nu}@{z}</t>
   </si>
   <si>
-    <t>X1X\LegendreBlackQ[\mu]{\nu}@{z}</t>
-  </si>
-  <si>
     <t>\FerrersHatQ{\tau}@{x}</t>
   </si>
   <si>
-    <t>X1X\FerrersHatQ[\mu]{\tau}@{x}</t>
-  </si>
-  <si>
-    <t>X1X\LegendreQ[$1]{$0}@{$2}</t>
-  </si>
-  <si>
-    <t>X1X\LegendreP[$1]{$0}@{$2}</t>
+    <t>LegendreP($1, $0, $2)*GAMMA(1-$0)</t>
+  </si>
+  <si>
+    <t>X1:\FerrersPX\FerrersP[\mu]{\nu}@{z}</t>
+  </si>
+  <si>
+    <t>X1:\FerrersQX\FerrersQ[\mu]{\nu}@{z}</t>
+  </si>
+  <si>
+    <t>X1:\LegendreQX\LegendreQ[$1]{$0}@{$2}</t>
+  </si>
+  <si>
+    <t>X1:\LegendreBlackQX\LegendreBlackQ[\mu]{\nu}@{z}</t>
+  </si>
+  <si>
+    <t>X1:\FerrersHatQX\FerrersHatQ[\mu]{\tau}@{x}</t>
+  </si>
+  <si>
+    <t>X1:\LegendrePX\frac{\LegendreP[$1]{$0}@{$2}{\EulerGamma{1-$1}}</t>
   </si>
 </sst>
 </file>
@@ -4064,14 +4064,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A390" workbookViewId="0">
-      <selection activeCell="D404" sqref="D404"/>
+    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
+      <selection activeCell="B402" sqref="B402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.08984375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="38.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="54.36328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" style="2" customWidth="1"/>
     <col min="4" max="5" width="32.453125" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.08984375" style="2" customWidth="1"/>
@@ -4093,10 +4093,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="37" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>1119</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>1120</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -4105,10 +4105,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -4517,7 +4517,7 @@
         <v>58</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>59</v>
@@ -4907,7 +4907,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="39" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="6" t="s">
@@ -4949,7 +4949,7 @@
     <row r="46" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
@@ -4957,7 +4957,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="6"/>
@@ -4965,7 +4965,7 @@
     <row r="47" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
@@ -4973,7 +4973,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="6"/>
@@ -5047,7 +5047,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="39" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="6" t="s">
@@ -5069,7 +5069,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="39" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="6" t="s">
@@ -5147,7 +5147,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="39" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="6" t="s">
@@ -6574,7 +6574,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="3" t="s">
         <v>281</v>
@@ -6590,7 +6590,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="3" t="s">
         <v>282</v>
@@ -7062,7 +7062,7 @@
       <c r="I162" s="5"/>
       <c r="J162" s="5"/>
     </row>
-    <row r="163" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
       <c r="B163" s="3" t="s">
         <v>317</v>
@@ -8196,7 +8196,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="232" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A232" s="5"/>
       <c r="B232" s="3" t="s">
         <v>394</v>
@@ -8872,7 +8872,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="274" spans="1:28" ht="27" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:28" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A274" s="5"/>
       <c r="B274" s="3" t="s">
         <v>446</v>
@@ -9654,7 +9654,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="317" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A317" s="5"/>
       <c r="B317" s="3" t="s">
         <v>518</v>
@@ -9732,7 +9732,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="322" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A322" s="3" t="s">
         <v>524</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="323" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A323" s="5"/>
       <c r="B323" s="3" t="s">
         <v>527</v>
@@ -9870,7 +9870,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="330" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A330" s="3" t="s">
         <v>542</v>
       </c>
@@ -9886,7 +9886,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="331" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A331" s="3" t="s">
         <v>544</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="332" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A332" s="5"/>
       <c r="B332" s="30" t="s">
         <v>546</v>
@@ -9930,7 +9930,7 @@
       <c r="I333" s="5"/>
       <c r="J333" s="5"/>
     </row>
-    <row r="334" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A334" s="3" t="s">
         <v>547</v>
       </c>
@@ -9990,7 +9990,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="337" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A337" s="5"/>
       <c r="B337" s="3" t="s">
         <v>555</v>
@@ -10144,7 +10144,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="345" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A345" s="5"/>
       <c r="B345" s="3" t="s">
         <v>573</v>
@@ -10872,7 +10872,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="382" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A382" s="5"/>
       <c r="B382" s="3" t="s">
         <v>639</v>
@@ -11125,7 +11125,7 @@
     <row r="397" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A397" s="3"/>
       <c r="B397" s="38" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C397" s="5"/>
       <c r="D397" s="5"/>
@@ -11139,7 +11139,7 @@
     <row r="398" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A398" s="3"/>
       <c r="B398" s="38" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="C398" s="5"/>
       <c r="D398" s="5"/>
@@ -11153,7 +11153,7 @@
     <row r="399" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A399" s="5"/>
       <c r="B399" s="38" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="C399" s="5"/>
       <c r="D399" s="5"/>
@@ -11167,7 +11167,7 @@
     <row r="400" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A400" s="5"/>
       <c r="B400" s="38" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="C400" s="5"/>
       <c r="D400" s="5"/>
@@ -11180,10 +11180,10 @@
     </row>
     <row r="401" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A401" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C401" s="5">
         <v>2</v>
@@ -11195,12 +11195,12 @@
       <c r="H401" s="38"/>
       <c r="I401" s="5"/>
       <c r="J401" s="6" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="402" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A402" s="3" t="s">
-        <v>662</v>
+        <v>1132</v>
       </c>
       <c r="B402" s="3" t="s">
         <v>1138</v>
@@ -11212,18 +11212,18 @@
       <c r="E402" s="3"/>
       <c r="F402" s="5"/>
       <c r="G402" s="5"/>
-      <c r="H402" s="38"/>
+      <c r="H402" s="3"/>
       <c r="I402" s="5"/>
       <c r="J402" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="403" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A403" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C403" s="5">
         <v>2</v>
@@ -11235,15 +11235,15 @@
       <c r="H403" s="38"/>
       <c r="I403" s="5"/>
       <c r="J403" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="404" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A404" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C404" s="5">
         <v>3</v>
@@ -11255,13 +11255,13 @@
       <c r="H404" s="38"/>
       <c r="I404" s="5"/>
       <c r="J404" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="405" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A405" s="5"/>
       <c r="B405" s="38" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="C405" s="5"/>
       <c r="D405" s="5"/>
@@ -11272,10 +11272,10 @@
       <c r="I405" s="5"/>
       <c r="J405" s="5"/>
     </row>
-    <row r="406" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A406" s="5"/>
       <c r="B406" s="38" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="C406" s="5"/>
       <c r="D406" s="5"/>
@@ -11289,7 +11289,7 @@
     <row r="407" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A407" s="5"/>
       <c r="B407" s="45" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="C407" s="5"/>
       <c r="D407" s="5"/>
@@ -11305,7 +11305,7 @@
     <row r="408" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A408" s="5"/>
       <c r="B408" s="45" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C408" s="5"/>
       <c r="D408" s="5"/>
@@ -11330,40 +11330,40 @@
     </row>
     <row r="410" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A410" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="B410" s="16" t="s">
         <v>666</v>
-      </c>
-      <c r="B410" s="16" t="s">
-        <v>667</v>
       </c>
       <c r="C410" s="21">
         <v>2</v>
       </c>
       <c r="D410" s="16" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E410" s="16"/>
       <c r="F410" s="5"/>
       <c r="G410" s="5"/>
       <c r="H410" s="39" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="I410" s="5"/>
       <c r="J410" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="411" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A411" s="16" t="s">
+        <v>669</v>
+      </c>
+      <c r="B411" s="16" t="s">
         <v>670</v>
-      </c>
-      <c r="B411" s="16" t="s">
-        <v>671</v>
       </c>
       <c r="C411" s="21">
         <v>2</v>
       </c>
       <c r="D411" s="16" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E411" s="16"/>
       <c r="F411" s="5"/>
@@ -11371,21 +11371,21 @@
       <c r="H411" s="38"/>
       <c r="I411" s="5"/>
       <c r="J411" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="412" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A412" s="16" t="s">
+        <v>672</v>
+      </c>
+      <c r="B412" s="16" t="s">
         <v>673</v>
-      </c>
-      <c r="B412" s="16" t="s">
-        <v>674</v>
       </c>
       <c r="C412" s="21">
         <v>3</v>
       </c>
       <c r="D412" s="16" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E412" s="16"/>
       <c r="F412" s="5"/>
@@ -11393,13 +11393,13 @@
       <c r="H412" s="38"/>
       <c r="I412" s="5"/>
       <c r="J412" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="413" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A413" s="5"/>
       <c r="B413" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C413" s="5"/>
       <c r="D413" s="3"/>
@@ -11414,10 +11414,10 @@
     </row>
     <row r="414" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A414" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="B414" s="3" t="s">
         <v>677</v>
-      </c>
-      <c r="B414" s="3" t="s">
-        <v>678</v>
       </c>
       <c r="C414" s="5">
         <v>1</v>
@@ -11427,19 +11427,19 @@
       <c r="F414" s="5"/>
       <c r="G414" s="5"/>
       <c r="H414" s="39" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="I414" s="5"/>
       <c r="J414" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="415" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A415" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="B415" s="3" t="s">
         <v>680</v>
-      </c>
-      <c r="B415" s="3" t="s">
-        <v>681</v>
       </c>
       <c r="C415" s="5">
         <v>1</v>
@@ -11451,15 +11451,15 @@
       <c r="H415" s="38"/>
       <c r="I415" s="5"/>
       <c r="J415" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="416" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A416" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B416" s="3" t="s">
         <v>682</v>
-      </c>
-      <c r="B416" s="3" t="s">
-        <v>683</v>
       </c>
       <c r="C416" s="5">
         <v>2</v>
@@ -11471,7 +11471,7 @@
       <c r="H416" s="38"/>
       <c r="I416" s="5"/>
       <c r="J416" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="417" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -11488,10 +11488,10 @@
     </row>
     <row r="418" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A418" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="B418" s="3" t="s">
         <v>684</v>
-      </c>
-      <c r="B418" s="3" t="s">
-        <v>685</v>
       </c>
       <c r="C418" s="5">
         <v>1</v>
@@ -11503,15 +11503,15 @@
       <c r="H418" s="38"/>
       <c r="I418" s="5"/>
       <c r="J418" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="419" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A419" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="B419" s="3" t="s">
         <v>687</v>
-      </c>
-      <c r="B419" s="3" t="s">
-        <v>688</v>
       </c>
       <c r="C419" s="5">
         <v>1</v>
@@ -11523,7 +11523,7 @@
       <c r="H419" s="38"/>
       <c r="I419" s="5"/>
       <c r="J419" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="420" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -11540,10 +11540,10 @@
     </row>
     <row r="421" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A421" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="B421" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="B421" s="3" t="s">
-        <v>691</v>
       </c>
       <c r="C421" s="5">
         <v>3</v>
@@ -11555,7 +11555,7 @@
       <c r="H421" s="38"/>
       <c r="I421" s="5"/>
       <c r="J421" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="422" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -11572,10 +11572,10 @@
     </row>
     <row r="423" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A423" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="B423" s="3" t="s">
         <v>693</v>
-      </c>
-      <c r="B423" s="3" t="s">
-        <v>694</v>
       </c>
       <c r="C423" s="5">
         <v>3</v>
@@ -11587,15 +11587,15 @@
       <c r="H423" s="38"/>
       <c r="I423" s="5"/>
       <c r="J423" s="6" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="424" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A424" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="B424" s="3" t="s">
         <v>696</v>
-      </c>
-      <c r="B424" s="3" t="s">
-        <v>697</v>
       </c>
       <c r="C424" s="5">
         <v>3</v>
@@ -11607,7 +11607,7 @@
       <c r="H424" s="38"/>
       <c r="I424" s="5"/>
       <c r="J424" s="6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="425" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -11624,10 +11624,10 @@
     </row>
     <row r="426" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A426" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="B426" s="3" t="s">
         <v>699</v>
-      </c>
-      <c r="B426" s="3" t="s">
-        <v>700</v>
       </c>
       <c r="C426" s="5">
         <v>2</v>
@@ -11637,19 +11637,19 @@
       <c r="F426" s="5"/>
       <c r="G426" s="5"/>
       <c r="H426" s="43" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I426" s="5"/>
       <c r="J426" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="427" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A427" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="B427" s="3" t="s">
         <v>702</v>
-      </c>
-      <c r="B427" s="3" t="s">
-        <v>703</v>
       </c>
       <c r="C427" s="5">
         <v>2</v>
@@ -11661,13 +11661,13 @@
       <c r="H427" s="38"/>
       <c r="I427" s="5"/>
       <c r="J427" s="6" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="428" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="428" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A428" s="5"/>
       <c r="B428" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C428" s="5"/>
       <c r="D428" s="5"/>
@@ -11682,34 +11682,34 @@
     </row>
     <row r="429" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A429" s="16" t="s">
+        <v>705</v>
+      </c>
+      <c r="B429" s="16" t="s">
         <v>706</v>
-      </c>
-      <c r="B429" s="16" t="s">
-        <v>707</v>
       </c>
       <c r="C429" s="21">
         <v>3</v>
       </c>
       <c r="D429" s="16" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E429" s="16"/>
       <c r="F429" s="21"/>
       <c r="G429" s="5"/>
       <c r="H429" s="38"/>
       <c r="I429" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="J429" s="6" t="s">
         <v>709</v>
-      </c>
-      <c r="J429" s="6" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="430" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A430" s="35" t="s">
+        <v>710</v>
+      </c>
+      <c r="B430" s="3" t="s">
         <v>711</v>
-      </c>
-      <c r="B430" s="3" t="s">
-        <v>712</v>
       </c>
       <c r="C430" s="5">
         <v>3</v>
@@ -11721,13 +11721,13 @@
       <c r="H430" s="38"/>
       <c r="I430" s="5"/>
       <c r="J430" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="431" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A431" s="36"/>
       <c r="B431" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C431" s="5"/>
       <c r="D431" s="5"/>
@@ -11741,7 +11741,7 @@
     <row r="432" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A432" s="5"/>
       <c r="B432" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C432" s="5"/>
       <c r="D432" s="5"/>
@@ -11757,7 +11757,7 @@
     <row r="433" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A433" s="5"/>
       <c r="B433" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C433" s="5"/>
       <c r="D433" s="5"/>
@@ -11773,7 +11773,7 @@
     <row r="434" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A434" s="5"/>
       <c r="B434" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C434" s="5"/>
       <c r="D434" s="5"/>
@@ -11789,7 +11789,7 @@
     <row r="435" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A435" s="5"/>
       <c r="B435" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C435" s="5"/>
       <c r="D435" s="5"/>
@@ -11805,7 +11805,7 @@
     <row r="436" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A436" s="5"/>
       <c r="B436" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C436" s="5"/>
       <c r="D436" s="5"/>
@@ -11821,7 +11821,7 @@
     <row r="437" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A437" s="5"/>
       <c r="B437" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C437" s="5"/>
       <c r="D437" s="5"/>
@@ -11837,7 +11837,7 @@
     <row r="438" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A438" s="5"/>
       <c r="B438" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C438" s="5"/>
       <c r="D438" s="5"/>
@@ -11853,7 +11853,7 @@
     <row r="439" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A439" s="5"/>
       <c r="B439" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C439" s="5"/>
       <c r="D439" s="5"/>
@@ -11869,7 +11869,7 @@
     <row r="440" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A440" s="5"/>
       <c r="B440" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C440" s="5"/>
       <c r="D440" s="5"/>
@@ -11885,7 +11885,7 @@
     <row r="441" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A441" s="5"/>
       <c r="B441" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C441" s="5"/>
       <c r="D441" s="5"/>
@@ -11901,7 +11901,7 @@
     <row r="442" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A442" s="5"/>
       <c r="B442" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C442" s="5"/>
       <c r="D442" s="5"/>
@@ -11917,7 +11917,7 @@
     <row r="443" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A443" s="5"/>
       <c r="B443" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C443" s="5"/>
       <c r="D443" s="5"/>
@@ -11933,7 +11933,7 @@
     <row r="444" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A444" s="5"/>
       <c r="B444" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C444" s="5"/>
       <c r="D444" s="5"/>
@@ -11949,7 +11949,7 @@
     <row r="445" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A445" s="5"/>
       <c r="B445" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C445" s="5"/>
       <c r="D445" s="5"/>
@@ -11965,7 +11965,7 @@
     <row r="446" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A446" s="5"/>
       <c r="B446" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C446" s="5"/>
       <c r="D446" s="5"/>
@@ -11981,7 +11981,7 @@
     <row r="447" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A447" s="5"/>
       <c r="B447" s="3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C447" s="5"/>
       <c r="D447" s="5"/>
@@ -11997,7 +11997,7 @@
     <row r="448" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A448" s="5"/>
       <c r="B448" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C448" s="5"/>
       <c r="D448" s="5"/>
@@ -12013,7 +12013,7 @@
     <row r="449" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A449" s="5"/>
       <c r="B449" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C449" s="5"/>
       <c r="D449" s="5"/>
@@ -12029,7 +12029,7 @@
     <row r="450" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A450" s="5"/>
       <c r="B450" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C450" s="5"/>
       <c r="D450" s="5"/>
@@ -12045,7 +12045,7 @@
     <row r="451" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A451" s="5"/>
       <c r="B451" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C451" s="5"/>
       <c r="D451" s="5"/>
@@ -12061,7 +12061,7 @@
     <row r="452" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A452" s="5"/>
       <c r="B452" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C452" s="5"/>
       <c r="D452" s="5"/>
@@ -12077,7 +12077,7 @@
     <row r="453" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A453" s="5"/>
       <c r="B453" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C453" s="5"/>
       <c r="D453" s="5"/>
@@ -12104,14 +12104,14 @@
     </row>
     <row r="455" spans="1:10" ht="67.5" x14ac:dyDescent="0.3">
       <c r="A455" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="B455" s="16" t="s">
         <v>737</v>
-      </c>
-      <c r="B455" s="16" t="s">
-        <v>738</v>
       </c>
       <c r="C455" s="21"/>
       <c r="D455" s="16" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E455" s="16"/>
       <c r="F455" s="5"/>
@@ -12119,7 +12119,7 @@
       <c r="H455" s="38"/>
       <c r="I455" s="5"/>
       <c r="J455" s="6" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="456" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -12137,11 +12137,11 @@
     <row r="457" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A457" s="5"/>
       <c r="B457" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C457" s="5"/>
       <c r="D457" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E457" s="3"/>
       <c r="F457" s="5"/>
@@ -12149,7 +12149,7 @@
       <c r="H457" s="38"/>
       <c r="I457" s="5"/>
       <c r="J457" s="6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="458" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -12167,7 +12167,7 @@
     <row r="459" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A459" s="5"/>
       <c r="B459" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C459" s="5"/>
       <c r="D459" s="5"/>
@@ -12183,7 +12183,7 @@
     <row r="460" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A460" s="5"/>
       <c r="B460" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C460" s="5"/>
       <c r="D460" s="5"/>
@@ -12227,7 +12227,7 @@
     <row r="463" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A463" s="5"/>
       <c r="B463" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C463" s="5"/>
       <c r="D463" s="5"/>
@@ -12255,7 +12255,7 @@
     <row r="465" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A465" s="5"/>
       <c r="B465" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C465" s="5"/>
       <c r="D465" s="5"/>
@@ -12271,7 +12271,7 @@
     <row r="466" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A466" s="5"/>
       <c r="B466" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C466" s="5"/>
       <c r="D466" s="5"/>
@@ -12299,7 +12299,7 @@
     <row r="468" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A468" s="5"/>
       <c r="B468" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C468" s="5"/>
       <c r="D468" s="5"/>
@@ -12326,30 +12326,30 @@
     </row>
     <row r="470" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A470" s="16" t="s">
+        <v>749</v>
+      </c>
+      <c r="B470" s="16" t="s">
         <v>750</v>
-      </c>
-      <c r="B470" s="16" t="s">
-        <v>751</v>
       </c>
       <c r="C470" s="21"/>
       <c r="D470" s="16" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E470" s="16"/>
       <c r="F470" s="5"/>
       <c r="G470" s="5"/>
       <c r="H470" s="39" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I470" s="5"/>
       <c r="J470" s="6" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="471" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="471" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A471" s="5"/>
       <c r="B471" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C471" s="5"/>
       <c r="D471" s="5"/>
@@ -12362,10 +12362,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="472" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A472" s="5"/>
       <c r="B472" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C472" s="5"/>
       <c r="D472" s="5"/>
@@ -12381,20 +12381,20 @@
     <row r="473" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A473" s="5"/>
       <c r="B473" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C473" s="5"/>
       <c r="D473" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E473" s="3"/>
       <c r="F473" s="25"/>
       <c r="G473" s="5"/>
       <c r="H473" s="39" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="I473" s="26" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J473" s="3" t="s">
         <v>199</v>
@@ -12402,10 +12402,10 @@
     </row>
     <row r="474" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A474" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="B474" s="3" t="s">
         <v>759</v>
-      </c>
-      <c r="B474" s="3" t="s">
-        <v>760</v>
       </c>
       <c r="C474" s="5">
         <v>1</v>
@@ -12415,11 +12415,11 @@
       <c r="F474" s="5"/>
       <c r="G474" s="5"/>
       <c r="H474" s="39" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I474" s="5"/>
       <c r="J474" s="6" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="475" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -12437,18 +12437,18 @@
     <row r="476" spans="1:10" ht="67.5" x14ac:dyDescent="0.3">
       <c r="A476" s="5"/>
       <c r="B476" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C476" s="5"/>
       <c r="D476" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E476" s="3"/>
       <c r="F476" s="25"/>
       <c r="G476" s="5"/>
       <c r="H476" s="38"/>
       <c r="I476" s="26" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="J476" s="3" t="s">
         <v>199</v>
@@ -12457,18 +12457,18 @@
     <row r="477" spans="1:10" ht="67.5" x14ac:dyDescent="0.3">
       <c r="A477" s="5"/>
       <c r="B477" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C477" s="5"/>
       <c r="D477" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E477" s="3"/>
       <c r="F477" s="25"/>
       <c r="G477" s="5"/>
       <c r="H477" s="38"/>
       <c r="I477" s="26" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="J477" s="3" t="s">
         <v>199</v>
@@ -12486,10 +12486,10 @@
       <c r="I478" s="5"/>
       <c r="J478" s="5"/>
     </row>
-    <row r="479" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A479" s="5"/>
       <c r="B479" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C479" s="5"/>
       <c r="D479" s="5"/>
@@ -12502,10 +12502,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="480" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A480" s="5"/>
       <c r="B480" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C480" s="5"/>
       <c r="D480" s="5"/>
@@ -12518,10 +12518,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="481" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A481" s="5"/>
       <c r="B481" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C481" s="5"/>
       <c r="D481" s="5"/>
@@ -12534,10 +12534,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="482" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A482" s="5"/>
       <c r="B482" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C482" s="5"/>
       <c r="D482" s="5"/>
@@ -12550,10 +12550,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="483" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A483" s="5"/>
       <c r="B483" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C483" s="5"/>
       <c r="D483" s="5"/>
@@ -12566,10 +12566,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="484" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A484" s="5"/>
       <c r="B484" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C484" s="5"/>
       <c r="D484" s="5"/>
@@ -12596,10 +12596,10 @@
     </row>
     <row r="486" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A486" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="B486" s="3" t="s">
         <v>773</v>
-      </c>
-      <c r="B486" s="3" t="s">
-        <v>774</v>
       </c>
       <c r="C486" s="5">
         <v>2</v>
@@ -12611,15 +12611,15 @@
       <c r="H486" s="38"/>
       <c r="I486" s="5"/>
       <c r="J486" s="6" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="487" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A487" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="B487" s="3" t="s">
         <v>776</v>
-      </c>
-      <c r="B487" s="3" t="s">
-        <v>777</v>
       </c>
       <c r="C487" s="5">
         <v>2</v>
@@ -12631,7 +12631,7 @@
       <c r="H487" s="38"/>
       <c r="I487" s="5"/>
       <c r="J487" s="6" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="488" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -12648,10 +12648,10 @@
     </row>
     <row r="489" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A489" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="B489" s="3" t="s">
         <v>779</v>
-      </c>
-      <c r="B489" s="3" t="s">
-        <v>780</v>
       </c>
       <c r="C489" s="5">
         <v>2</v>
@@ -12663,13 +12663,13 @@
       <c r="H489" s="38"/>
       <c r="I489" s="5"/>
       <c r="J489" s="6" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="490" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A490" s="5"/>
       <c r="B490" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C490" s="5"/>
       <c r="D490" s="5"/>
@@ -12684,10 +12684,10 @@
     </row>
     <row r="491" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A491" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="B491" s="3" t="s">
         <v>783</v>
-      </c>
-      <c r="B491" s="3" t="s">
-        <v>784</v>
       </c>
       <c r="C491" s="5">
         <v>2</v>
@@ -12699,13 +12699,13 @@
       <c r="H491" s="44"/>
       <c r="I491" s="5"/>
       <c r="J491" s="6" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="492" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A492" s="5"/>
       <c r="B492" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C492" s="5"/>
       <c r="D492" s="5"/>
@@ -12732,16 +12732,16 @@
     </row>
     <row r="494" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A494" s="17" t="s">
+        <v>786</v>
+      </c>
+      <c r="B494" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="B494" s="3" t="s">
-        <v>788</v>
       </c>
       <c r="C494" s="5">
         <v>2</v>
       </c>
       <c r="D494" s="17" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E494" s="17"/>
       <c r="F494" s="5"/>
@@ -12749,21 +12749,21 @@
       <c r="H494" s="44"/>
       <c r="I494" s="5"/>
       <c r="J494" s="6" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="495" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A495" s="17" t="s">
+        <v>790</v>
+      </c>
+      <c r="B495" s="3" t="s">
         <v>791</v>
-      </c>
-      <c r="B495" s="3" t="s">
-        <v>792</v>
       </c>
       <c r="C495" s="5">
         <v>2</v>
       </c>
       <c r="D495" s="17" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E495" s="17"/>
       <c r="F495" s="5"/>
@@ -12771,19 +12771,19 @@
       <c r="H495" s="38"/>
       <c r="I495" s="5"/>
       <c r="J495" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="496" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A496" s="17" t="s">
+        <v>794</v>
+      </c>
+      <c r="B496" s="3" t="s">
         <v>795</v>
-      </c>
-      <c r="B496" s="3" t="s">
-        <v>796</v>
       </c>
       <c r="C496" s="5"/>
       <c r="D496" s="17" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E496" s="17"/>
       <c r="F496" s="5"/>
@@ -12796,16 +12796,16 @@
     </row>
     <row r="497" spans="1:10" ht="67.5" x14ac:dyDescent="0.3">
       <c r="A497" s="17" t="s">
+        <v>796</v>
+      </c>
+      <c r="B497" s="3" t="s">
         <v>797</v>
-      </c>
-      <c r="B497" s="3" t="s">
-        <v>798</v>
       </c>
       <c r="C497" s="5">
         <v>3</v>
       </c>
       <c r="D497" s="17" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E497" s="17"/>
       <c r="F497" s="5"/>
@@ -12813,10 +12813,10 @@
       <c r="H497" s="38"/>
       <c r="I497" s="5"/>
       <c r="J497" s="6" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="498" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="498" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A498" s="5"/>
       <c r="B498" s="3" t="s">
         <v>573</v>
@@ -12834,10 +12834,10 @@
     </row>
     <row r="499" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A499" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="B499" s="3" t="s">
         <v>801</v>
-      </c>
-      <c r="B499" s="3" t="s">
-        <v>802</v>
       </c>
       <c r="C499" s="5">
         <v>2</v>
@@ -12849,13 +12849,13 @@
       <c r="H499" s="38"/>
       <c r="I499" s="5"/>
       <c r="J499" s="6" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="500" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="500" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A500" s="5"/>
       <c r="B500" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C500" s="5"/>
       <c r="D500" s="5"/>
@@ -12871,7 +12871,7 @@
     <row r="501" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A501" s="5"/>
       <c r="B501" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C501" s="5"/>
       <c r="D501" s="5"/>
@@ -12884,10 +12884,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="502" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A502" s="5"/>
       <c r="B502" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C502" s="5"/>
       <c r="D502" s="5"/>
@@ -12903,7 +12903,7 @@
     <row r="503" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A503" s="5"/>
       <c r="B503" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C503" s="5"/>
       <c r="D503" s="5"/>
@@ -12911,7 +12911,7 @@
       <c r="F503" s="5"/>
       <c r="G503" s="5"/>
       <c r="H503" s="39" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I503" s="5"/>
       <c r="J503" s="3" t="s">
@@ -12933,7 +12933,7 @@
     <row r="505" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A505" s="5"/>
       <c r="B505" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C505" s="5"/>
       <c r="D505" s="5"/>
@@ -12949,7 +12949,7 @@
     <row r="506" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A506" s="5"/>
       <c r="B506" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C506" s="5"/>
       <c r="D506" s="5"/>
@@ -12958,7 +12958,7 @@
       <c r="G506" s="5"/>
       <c r="H506" s="38"/>
       <c r="I506" s="26" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="J506" s="3" t="s">
         <v>199</v>
@@ -12978,14 +12978,14 @@
     </row>
     <row r="508" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A508" s="17" t="s">
+        <v>810</v>
+      </c>
+      <c r="B508" s="3" t="s">
         <v>811</v>
-      </c>
-      <c r="B508" s="3" t="s">
-        <v>812</v>
       </c>
       <c r="C508" s="5"/>
       <c r="D508" s="17" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E508" s="17"/>
       <c r="F508" s="5"/>
@@ -12993,19 +12993,19 @@
       <c r="H508" s="38"/>
       <c r="I508" s="5"/>
       <c r="J508" s="6" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="509" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A509" s="17" t="s">
+        <v>814</v>
+      </c>
+      <c r="B509" s="3" t="s">
         <v>815</v>
-      </c>
-      <c r="B509" s="3" t="s">
-        <v>816</v>
       </c>
       <c r="C509" s="5"/>
       <c r="D509" s="17" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E509" s="17"/>
       <c r="F509" s="5"/>
@@ -13013,19 +13013,19 @@
       <c r="H509" s="38"/>
       <c r="I509" s="5"/>
       <c r="J509" s="6" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="510" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A510" s="17" t="s">
+        <v>817</v>
+      </c>
+      <c r="B510" s="3" t="s">
         <v>818</v>
-      </c>
-      <c r="B510" s="3" t="s">
-        <v>819</v>
       </c>
       <c r="C510" s="5"/>
       <c r="D510" s="17" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E510" s="17"/>
       <c r="F510" s="5"/>
@@ -13033,19 +13033,19 @@
       <c r="H510" s="38"/>
       <c r="I510" s="5"/>
       <c r="J510" s="6" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="511" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A511" s="17" t="s">
+        <v>820</v>
+      </c>
+      <c r="B511" s="3" t="s">
         <v>821</v>
-      </c>
-      <c r="B511" s="3" t="s">
-        <v>822</v>
       </c>
       <c r="C511" s="5"/>
       <c r="D511" s="17" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E511" s="17"/>
       <c r="F511" s="5"/>
@@ -13053,13 +13053,13 @@
       <c r="H511" s="38"/>
       <c r="I511" s="5"/>
       <c r="J511" s="6" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="512" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A512" s="5"/>
       <c r="B512" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C512" s="5"/>
       <c r="D512" s="5"/>
@@ -13087,7 +13087,7 @@
     <row r="514" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A514" s="5"/>
       <c r="B514" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C514" s="5"/>
       <c r="D514" s="5"/>
@@ -13114,16 +13114,16 @@
     </row>
     <row r="516" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A516" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B516" s="3" t="s">
         <v>826</v>
-      </c>
-      <c r="B516" s="3" t="s">
-        <v>827</v>
       </c>
       <c r="C516" s="5">
         <v>1</v>
       </c>
       <c r="D516" s="17" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E516" s="17"/>
       <c r="F516" s="5"/>
@@ -13131,21 +13131,21 @@
       <c r="H516" s="38"/>
       <c r="I516" s="5"/>
       <c r="J516" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="517" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A517" s="17" t="s">
+        <v>829</v>
+      </c>
+      <c r="B517" s="3" t="s">
         <v>830</v>
-      </c>
-      <c r="B517" s="3" t="s">
-        <v>831</v>
       </c>
       <c r="C517" s="5">
         <v>1</v>
       </c>
       <c r="D517" s="17" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E517" s="17"/>
       <c r="F517" s="5"/>
@@ -13153,21 +13153,21 @@
       <c r="H517" s="38"/>
       <c r="I517" s="5"/>
       <c r="J517" s="6" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="518" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A518" s="17" t="s">
+        <v>832</v>
+      </c>
+      <c r="B518" s="3" t="s">
         <v>833</v>
-      </c>
-      <c r="B518" s="3" t="s">
-        <v>834</v>
       </c>
       <c r="C518" s="5">
         <v>1</v>
       </c>
       <c r="D518" s="17" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E518" s="17"/>
       <c r="F518" s="5"/>
@@ -13175,7 +13175,7 @@
       <c r="H518" s="38"/>
       <c r="I518" s="5"/>
       <c r="J518" s="6" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="519" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -13193,7 +13193,7 @@
     <row r="520" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A520" s="5"/>
       <c r="B520" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C520" s="5"/>
       <c r="D520" s="5"/>
@@ -13209,7 +13209,7 @@
     <row r="521" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A521" s="5"/>
       <c r="B521" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C521" s="5"/>
       <c r="D521" s="5"/>
@@ -13225,7 +13225,7 @@
     <row r="522" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A522" s="5"/>
       <c r="B522" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C522" s="5"/>
       <c r="D522" s="5"/>
@@ -13253,7 +13253,7 @@
     <row r="524" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A524" s="5"/>
       <c r="B524" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C524" s="5"/>
       <c r="D524" s="5"/>
@@ -13269,7 +13269,7 @@
     <row r="525" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A525" s="5"/>
       <c r="B525" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C525" s="5"/>
       <c r="D525" s="5"/>
@@ -13285,7 +13285,7 @@
     <row r="526" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A526" s="5"/>
       <c r="B526" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C526" s="5"/>
       <c r="D526" s="5"/>
@@ -13310,12 +13310,12 @@
       <c r="I527" s="5"/>
       <c r="J527" s="5"/>
     </row>
-    <row r="528" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A528" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="B528" s="3" t="s">
         <v>842</v>
-      </c>
-      <c r="B528" s="3" t="s">
-        <v>843</v>
       </c>
       <c r="C528" s="5">
         <v>3</v>
@@ -13327,13 +13327,13 @@
       <c r="H528" s="38"/>
       <c r="I528" s="5"/>
       <c r="J528" s="6" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="529" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A529" s="5"/>
       <c r="B529" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C529" s="5"/>
       <c r="D529" s="5"/>
@@ -13348,10 +13348,10 @@
     </row>
     <row r="530" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A530" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B530" s="3" t="s">
         <v>846</v>
-      </c>
-      <c r="B530" s="3" t="s">
-        <v>847</v>
       </c>
       <c r="C530" s="5">
         <v>3</v>
@@ -13363,13 +13363,13 @@
       <c r="H530" s="38"/>
       <c r="I530" s="5"/>
       <c r="J530" s="6" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="531" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A531" s="5"/>
       <c r="B531" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C531" s="5"/>
       <c r="D531" s="5"/>
@@ -13384,10 +13384,10 @@
     </row>
     <row r="532" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A532" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="B532" s="3" t="s">
         <v>850</v>
-      </c>
-      <c r="B532" s="3" t="s">
-        <v>851</v>
       </c>
       <c r="C532" s="5">
         <v>3</v>
@@ -13399,13 +13399,13 @@
       <c r="H532" s="38"/>
       <c r="I532" s="5"/>
       <c r="J532" s="6" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="533" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A533" s="5"/>
       <c r="B533" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C533" s="5"/>
       <c r="D533" s="5"/>
@@ -13432,10 +13432,10 @@
     </row>
     <row r="535" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A535" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="B535" s="3" t="s">
         <v>854</v>
-      </c>
-      <c r="B535" s="3" t="s">
-        <v>855</v>
       </c>
       <c r="C535" s="5">
         <v>3</v>
@@ -13447,15 +13447,15 @@
       <c r="H535" s="38"/>
       <c r="I535" s="5"/>
       <c r="J535" s="6" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="536" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A536" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="B536" s="3" t="s">
         <v>857</v>
-      </c>
-      <c r="B536" s="3" t="s">
-        <v>858</v>
       </c>
       <c r="C536" s="5">
         <v>3</v>
@@ -13467,7 +13467,7 @@
       <c r="H536" s="38"/>
       <c r="I536" s="5"/>
       <c r="J536" s="6" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="537" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -13484,10 +13484,10 @@
     </row>
     <row r="538" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A538" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B538" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C538" s="5">
         <v>1</v>
@@ -13499,15 +13499,15 @@
       <c r="H538" s="38"/>
       <c r="I538" s="5"/>
       <c r="J538" s="6" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="539" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A539" s="16" t="s">
+        <v>860</v>
+      </c>
+      <c r="B539" s="16" t="s">
         <v>861</v>
-      </c>
-      <c r="B539" s="16" t="s">
-        <v>862</v>
       </c>
       <c r="C539" s="21">
         <v>3</v>
@@ -13519,15 +13519,15 @@
       <c r="H539" s="38"/>
       <c r="I539" s="5"/>
       <c r="J539" s="6" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="540" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A540" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B540" s="3" t="s">
         <v>846</v>
-      </c>
-      <c r="B540" s="3" t="s">
-        <v>847</v>
       </c>
       <c r="C540" s="5">
         <v>3</v>
@@ -13539,13 +13539,13 @@
       <c r="H540" s="38"/>
       <c r="I540" s="5"/>
       <c r="J540" s="6" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="541" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A541" s="5"/>
       <c r="B541" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C541" s="5"/>
       <c r="D541" s="5"/>
@@ -13581,7 +13581,7 @@
     <row r="543" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A543" s="5"/>
       <c r="B543" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C543" s="5"/>
       <c r="D543" s="5"/>
@@ -13606,10 +13606,10 @@
       <c r="I544" s="5"/>
       <c r="J544" s="5"/>
     </row>
-    <row r="545" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A545" s="5"/>
       <c r="B545" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C545" s="5"/>
       <c r="D545" s="5"/>
@@ -13622,10 +13622,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="546" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A546" s="5"/>
       <c r="B546" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C546" s="5"/>
       <c r="D546" s="5"/>
@@ -13638,10 +13638,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="547" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A547" s="5"/>
       <c r="B547" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C547" s="5"/>
       <c r="D547" s="5"/>
@@ -13657,7 +13657,7 @@
     <row r="548" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A548" s="5"/>
       <c r="B548" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C548" s="5"/>
       <c r="D548" s="5"/>
@@ -13673,7 +13673,7 @@
     <row r="549" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A549" s="5"/>
       <c r="B549" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C549" s="5"/>
       <c r="D549" s="5"/>
@@ -13689,7 +13689,7 @@
     <row r="550" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A550" s="5"/>
       <c r="B550" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C550" s="5"/>
       <c r="D550" s="5"/>
@@ -13714,10 +13714,10 @@
       <c r="I551" s="5"/>
       <c r="J551" s="5"/>
     </row>
-    <row r="552" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A552" s="5"/>
       <c r="B552" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C552" s="5"/>
       <c r="D552" s="5"/>
@@ -13730,10 +13730,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="553" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A553" s="5"/>
       <c r="B553" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C553" s="5"/>
       <c r="D553" s="5"/>
@@ -13760,16 +13760,16 @@
     </row>
     <row r="555" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A555" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="B555" s="3" t="s">
         <v>872</v>
-      </c>
-      <c r="B555" s="3" t="s">
-        <v>873</v>
       </c>
       <c r="C555" s="5">
         <v>2</v>
       </c>
       <c r="D555" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E555" s="3"/>
       <c r="F555" s="5"/>
@@ -13777,13 +13777,13 @@
       <c r="H555" s="38"/>
       <c r="I555" s="5"/>
       <c r="J555" s="6" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="556" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A556" s="5"/>
       <c r="B556" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C556" s="5"/>
       <c r="D556" s="5"/>
@@ -13799,7 +13799,7 @@
     <row r="557" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A557" s="5"/>
       <c r="B557" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C557" s="5"/>
       <c r="D557" s="5"/>
@@ -13807,7 +13807,7 @@
       <c r="F557" s="5"/>
       <c r="G557" s="5"/>
       <c r="H557" s="38" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I557" s="5"/>
       <c r="J557" s="3" t="s">
@@ -13817,7 +13817,7 @@
     <row r="558" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A558" s="5"/>
       <c r="B558" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C558" s="5"/>
       <c r="D558" s="5"/>
@@ -13844,26 +13844,26 @@
     </row>
     <row r="560" spans="1:10" ht="81" x14ac:dyDescent="0.3">
       <c r="A560" s="16" t="s">
+        <v>878</v>
+      </c>
+      <c r="B560" s="16" t="s">
         <v>879</v>
-      </c>
-      <c r="B560" s="16" t="s">
-        <v>880</v>
       </c>
       <c r="C560" s="21">
         <v>2</v>
       </c>
       <c r="D560" s="16" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E560" s="16"/>
       <c r="F560" s="5"/>
       <c r="G560" s="5"/>
       <c r="H560" s="38"/>
       <c r="I560" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="J560" s="6" t="s">
         <v>882</v>
-      </c>
-      <c r="J560" s="6" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="561" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -13881,7 +13881,7 @@
     <row r="562" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A562" s="5"/>
       <c r="B562" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C562" s="5"/>
       <c r="D562" s="5"/>
@@ -13897,7 +13897,7 @@
     <row r="563" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A563" s="5"/>
       <c r="B563" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C563" s="5"/>
       <c r="D563" s="5"/>
@@ -13913,7 +13913,7 @@
     <row r="564" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A564" s="5"/>
       <c r="B564" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C564" s="5"/>
       <c r="D564" s="5"/>
@@ -13929,7 +13929,7 @@
     <row r="565" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A565" s="5"/>
       <c r="B565" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C565" s="5"/>
       <c r="D565" s="5"/>
@@ -13957,7 +13957,7 @@
     <row r="567" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A567" s="5"/>
       <c r="B567" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C567" s="5"/>
       <c r="D567" s="5"/>
@@ -13973,7 +13973,7 @@
     <row r="568" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A568" s="5"/>
       <c r="B568" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C568" s="5"/>
       <c r="D568" s="5"/>
@@ -14000,10 +14000,10 @@
     </row>
     <row r="570" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A570" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="B570" s="3" t="s">
         <v>890</v>
-      </c>
-      <c r="B570" s="3" t="s">
-        <v>891</v>
       </c>
       <c r="C570" s="5">
         <v>2</v>
@@ -14015,15 +14015,15 @@
       <c r="H570" s="38"/>
       <c r="I570" s="5"/>
       <c r="J570" s="6" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="571" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A571" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="B571" s="3" t="s">
         <v>893</v>
-      </c>
-      <c r="B571" s="3" t="s">
-        <v>894</v>
       </c>
       <c r="C571" s="5">
         <v>2</v>
@@ -14035,13 +14035,13 @@
       <c r="H571" s="38"/>
       <c r="I571" s="5"/>
       <c r="J571" s="6" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="572" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A572" s="5"/>
       <c r="B572" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C572" s="5"/>
       <c r="D572" s="5"/>
@@ -14057,7 +14057,7 @@
     <row r="573" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A573" s="5"/>
       <c r="B573" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C573" s="5"/>
       <c r="D573" s="5"/>
@@ -14073,7 +14073,7 @@
     <row r="574" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A574" s="5"/>
       <c r="B574" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C574" s="5"/>
       <c r="D574" s="5"/>
@@ -14089,7 +14089,7 @@
     <row r="575" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A575" s="5"/>
       <c r="B575" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C575" s="5"/>
       <c r="D575" s="5"/>
@@ -14105,7 +14105,7 @@
     <row r="576" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A576" s="5"/>
       <c r="B576" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C576" s="5"/>
       <c r="D576" s="5"/>
@@ -14121,7 +14121,7 @@
     <row r="577" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A577" s="5"/>
       <c r="B577" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C577" s="5"/>
       <c r="D577" s="5"/>
@@ -14137,7 +14137,7 @@
     <row r="578" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A578" s="5"/>
       <c r="B578" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C578" s="5"/>
       <c r="D578" s="5"/>
@@ -14153,7 +14153,7 @@
     <row r="579" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A579" s="5"/>
       <c r="B579" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C579" s="5"/>
       <c r="D579" s="5"/>
@@ -14169,7 +14169,7 @@
     <row r="580" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A580" s="5"/>
       <c r="B580" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C580" s="5"/>
       <c r="D580" s="5"/>
@@ -14185,7 +14185,7 @@
     <row r="581" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A581" s="5"/>
       <c r="B581" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C581" s="5"/>
       <c r="D581" s="5"/>
@@ -14213,7 +14213,7 @@
     <row r="583" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A583" s="5"/>
       <c r="B583" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C583" s="5"/>
       <c r="D583" s="5"/>
@@ -14240,10 +14240,10 @@
     </row>
     <row r="585" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A585" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="B585" s="3" t="s">
         <v>907</v>
-      </c>
-      <c r="B585" s="3" t="s">
-        <v>908</v>
       </c>
       <c r="C585" s="5">
         <v>2</v>
@@ -14255,13 +14255,13 @@
       <c r="H585" s="38"/>
       <c r="I585" s="5"/>
       <c r="J585" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="586" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A586" s="5"/>
       <c r="B586" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C586" s="5"/>
       <c r="D586" s="5"/>
@@ -14277,7 +14277,7 @@
     <row r="587" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A587" s="5"/>
       <c r="B587" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C587" s="5"/>
       <c r="D587" s="5"/>
@@ -14302,12 +14302,12 @@
       <c r="I588" s="5"/>
       <c r="J588" s="5"/>
     </row>
-    <row r="589" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A589" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="B589" s="3" t="s">
         <v>912</v>
-      </c>
-      <c r="B589" s="3" t="s">
-        <v>913</v>
       </c>
       <c r="C589" s="5">
         <v>3</v>
@@ -14319,15 +14319,15 @@
       <c r="H589" s="38"/>
       <c r="I589" s="5"/>
       <c r="J589" s="6" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="590" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A590" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="B590" s="3" t="s">
         <v>914</v>
-      </c>
-    </row>
-    <row r="590" spans="1:10" ht="27" x14ac:dyDescent="0.3">
-      <c r="A590" s="3" t="s">
-        <v>912</v>
-      </c>
-      <c r="B590" s="3" t="s">
-        <v>915</v>
       </c>
       <c r="C590" s="5">
         <v>3</v>
@@ -14339,13 +14339,13 @@
       <c r="H590" s="38"/>
       <c r="I590" s="5"/>
       <c r="J590" s="6" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="591" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="591" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A591" s="5"/>
       <c r="B591" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C591" s="5"/>
       <c r="D591" s="5"/>
@@ -14373,7 +14373,7 @@
     <row r="593" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A593" s="5"/>
       <c r="B593" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C593" s="5"/>
       <c r="D593" s="5"/>
@@ -14386,10 +14386,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="594" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A594" s="5"/>
       <c r="B594" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C594" s="5"/>
       <c r="D594" s="5"/>
@@ -14402,10 +14402,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="595" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A595" s="5"/>
       <c r="B595" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C595" s="5"/>
       <c r="D595" s="5"/>
@@ -14418,10 +14418,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="596" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A596" s="5"/>
       <c r="B596" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C596" s="5"/>
       <c r="D596" s="5"/>
@@ -14437,7 +14437,7 @@
     <row r="597" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A597" s="5"/>
       <c r="B597" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C597" s="5"/>
       <c r="D597" s="5"/>
@@ -14450,10 +14450,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="598" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A598" s="5"/>
       <c r="B598" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C598" s="5"/>
       <c r="D598" s="5"/>
@@ -14480,10 +14480,10 @@
     </row>
     <row r="600" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A600" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="B600" s="3" t="s">
         <v>923</v>
-      </c>
-      <c r="B600" s="3" t="s">
-        <v>924</v>
       </c>
       <c r="C600" s="5">
         <v>2</v>
@@ -14495,15 +14495,15 @@
       <c r="H600" s="38"/>
       <c r="I600" s="5"/>
       <c r="J600" s="6" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="601" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A601" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B601" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C601" s="5">
         <v>2</v>
@@ -14515,13 +14515,13 @@
       <c r="H601" s="38"/>
       <c r="I601" s="5"/>
       <c r="J601" s="6" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="602" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A602" s="5"/>
       <c r="B602" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C602" s="5"/>
       <c r="D602" s="5"/>
@@ -14537,7 +14537,7 @@
     <row r="603" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A603" s="5"/>
       <c r="B603" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C603" s="5"/>
       <c r="D603" s="5"/>
@@ -14565,7 +14565,7 @@
     <row r="605" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A605" s="5"/>
       <c r="B605" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C605" s="5"/>
       <c r="D605" s="5"/>
@@ -14587,17 +14587,17 @@
       <c r="F606" s="5"/>
       <c r="G606" s="5"/>
       <c r="H606" s="39" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="I606" s="5"/>
       <c r="J606" s="5"/>
     </row>
     <row r="607" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A607" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="B607" s="3" t="s">
         <v>930</v>
-      </c>
-      <c r="B607" s="3" t="s">
-        <v>931</v>
       </c>
       <c r="C607" s="5">
         <v>4</v>
@@ -14609,15 +14609,15 @@
       <c r="H607" s="38"/>
       <c r="I607" s="5"/>
       <c r="J607" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="608" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A608" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B608" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C608" s="5">
         <v>4</v>
@@ -14629,13 +14629,13 @@
       <c r="H608" s="38"/>
       <c r="I608" s="5"/>
       <c r="J608" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="609" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A609" s="5"/>
       <c r="B609" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C609" s="5"/>
       <c r="D609" s="5"/>
@@ -14644,16 +14644,16 @@
       <c r="G609" s="5"/>
       <c r="H609" s="38"/>
       <c r="I609" s="26" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="J609" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="610" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="610" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A610" s="5"/>
       <c r="B610" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C610" s="5"/>
       <c r="D610" s="5"/>
@@ -14669,7 +14669,7 @@
     <row r="611" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A611" s="5"/>
       <c r="B611" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C611" s="5"/>
       <c r="D611" s="5"/>
@@ -14682,10 +14682,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="612" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="612" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A612" s="5"/>
       <c r="B612" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C612" s="5"/>
       <c r="D612" s="5"/>
@@ -14713,7 +14713,7 @@
     <row r="614" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A614" s="5"/>
       <c r="B614" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C614" s="5"/>
       <c r="D614" s="5"/>
@@ -14729,7 +14729,7 @@
     <row r="615" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A615" s="5"/>
       <c r="B615" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C615" s="5"/>
       <c r="D615" s="5"/>
@@ -14756,10 +14756,10 @@
     </row>
     <row r="617" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A617" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="B617" s="3" t="s">
         <v>941</v>
-      </c>
-      <c r="B617" s="3" t="s">
-        <v>942</v>
       </c>
       <c r="C617" s="5">
         <v>3</v>
@@ -14770,16 +14770,16 @@
       <c r="G617" s="5"/>
       <c r="H617" s="38"/>
       <c r="I617" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="J617" s="6" t="s">
         <v>943</v>
-      </c>
-      <c r="J617" s="6" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="618" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A618" s="5"/>
       <c r="B618" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C618" s="5"/>
       <c r="D618" s="5"/>
@@ -14807,7 +14807,7 @@
     <row r="620" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A620" s="5"/>
       <c r="B620" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C620" s="5"/>
       <c r="D620" s="5"/>
@@ -14823,7 +14823,7 @@
     <row r="621" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A621" s="5"/>
       <c r="B621" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C621" s="5"/>
       <c r="D621" s="5"/>
@@ -14839,7 +14839,7 @@
     <row r="622" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A622" s="5"/>
       <c r="B622" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C622" s="5"/>
       <c r="D622" s="5"/>
@@ -14855,7 +14855,7 @@
     <row r="623" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A623" s="5"/>
       <c r="B623" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C623" s="5"/>
       <c r="D623" s="5"/>
@@ -14871,7 +14871,7 @@
     <row r="624" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A624" s="5"/>
       <c r="B624" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C624" s="5"/>
       <c r="D624" s="5"/>
@@ -14887,7 +14887,7 @@
     <row r="625" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A625" s="5"/>
       <c r="B625" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C625" s="5"/>
       <c r="D625" s="5"/>
@@ -14903,7 +14903,7 @@
     <row r="626" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A626" s="5"/>
       <c r="B626" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C626" s="5"/>
       <c r="D626" s="5"/>
@@ -14919,7 +14919,7 @@
     <row r="627" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A627" s="5"/>
       <c r="B627" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C627" s="5"/>
       <c r="D627" s="5"/>
@@ -14946,16 +14946,16 @@
     </row>
     <row r="629" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A629" s="17" t="s">
+        <v>953</v>
+      </c>
+      <c r="B629" s="3" t="s">
         <v>954</v>
-      </c>
-      <c r="B629" s="3" t="s">
-        <v>955</v>
       </c>
       <c r="C629" s="5">
         <v>2</v>
       </c>
       <c r="D629" s="17" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E629" s="17"/>
       <c r="F629" s="5"/>
@@ -14969,7 +14969,7 @@
     <row r="630" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A630" s="5"/>
       <c r="B630" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C630" s="5"/>
       <c r="D630" s="5"/>
@@ -14985,7 +14985,7 @@
     <row r="631" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A631" s="5"/>
       <c r="B631" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C631" s="5"/>
       <c r="D631" s="5"/>
@@ -15013,7 +15013,7 @@
     <row r="633" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A633" s="5"/>
       <c r="B633" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C633" s="5"/>
       <c r="D633" s="5"/>
@@ -15029,7 +15029,7 @@
     <row r="634" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A634" s="5"/>
       <c r="B634" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C634" s="5"/>
       <c r="D634" s="5"/>
@@ -15042,10 +15042,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="635" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="635" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A635" s="5"/>
       <c r="B635" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C635" s="5"/>
       <c r="D635" s="5"/>
@@ -15058,10 +15058,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="636" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A636" s="5"/>
       <c r="B636" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C636" s="5"/>
       <c r="D636" s="5"/>
@@ -15089,7 +15089,7 @@
     <row r="638" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A638" s="5"/>
       <c r="B638" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C638" s="5"/>
       <c r="D638" s="5"/>
@@ -15114,10 +15114,10 @@
       <c r="I639" s="5"/>
       <c r="J639" s="5"/>
     </row>
-    <row r="640" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="640" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A640" s="5"/>
       <c r="B640" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C640" s="5"/>
       <c r="D640" s="5"/>
@@ -15142,10 +15142,10 @@
       <c r="I641" s="5"/>
       <c r="J641" s="5"/>
     </row>
-    <row r="642" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="642" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A642" s="5"/>
       <c r="B642" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C642" s="5"/>
       <c r="D642" s="5"/>
@@ -15158,10 +15158,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="643" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="643" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A643" s="5"/>
       <c r="B643" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C643" s="5"/>
       <c r="D643" s="5"/>
@@ -15189,7 +15189,7 @@
     <row r="645" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A645" s="5"/>
       <c r="B645" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C645" s="5"/>
       <c r="D645" s="5"/>
@@ -15205,7 +15205,7 @@
     <row r="646" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A646" s="5"/>
       <c r="B646" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C646" s="5"/>
       <c r="D646" s="5"/>
@@ -15233,7 +15233,7 @@
     <row r="648" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A648" s="5"/>
       <c r="B648" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C648" s="5"/>
       <c r="D648" s="5"/>
@@ -15249,7 +15249,7 @@
     <row r="649" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A649" s="5"/>
       <c r="B649" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C649" s="5"/>
       <c r="D649" s="5"/>
@@ -15277,7 +15277,7 @@
     <row r="651" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A651" s="5"/>
       <c r="B651" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C651" s="5"/>
       <c r="D651" s="5"/>
@@ -15353,11 +15353,11 @@
     <row r="656" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A656" s="5"/>
       <c r="B656" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C656" s="5"/>
       <c r="D656" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E656" s="3"/>
       <c r="F656" s="5"/>
@@ -15371,11 +15371,11 @@
     <row r="657" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A657" s="5"/>
       <c r="B657" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C657" s="5"/>
       <c r="D657" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E657" s="3"/>
       <c r="F657" s="5"/>
@@ -15389,11 +15389,11 @@
     <row r="658" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A658" s="5"/>
       <c r="B658" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C658" s="5"/>
       <c r="D658" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E658" s="3"/>
       <c r="F658" s="5"/>
@@ -15407,11 +15407,11 @@
     <row r="659" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A659" s="5"/>
       <c r="B659" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C659" s="5"/>
       <c r="D659" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E659" s="3"/>
       <c r="F659" s="5"/>
@@ -15425,11 +15425,11 @@
     <row r="660" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A660" s="5"/>
       <c r="B660" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C660" s="5"/>
       <c r="D660" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E660" s="3"/>
       <c r="F660" s="5"/>
@@ -15443,11 +15443,11 @@
     <row r="661" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A661" s="5"/>
       <c r="B661" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C661" s="5"/>
       <c r="D661" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E661" s="3"/>
       <c r="F661" s="5"/>
@@ -15461,11 +15461,11 @@
     <row r="662" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A662" s="5"/>
       <c r="B662" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C662" s="5"/>
       <c r="D662" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E662" s="3"/>
       <c r="F662" s="5"/>
@@ -15479,11 +15479,11 @@
     <row r="663" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A663" s="5"/>
       <c r="B663" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C663" s="5"/>
       <c r="D663" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E663" s="3"/>
       <c r="F663" s="5"/>
@@ -15497,11 +15497,11 @@
     <row r="664" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A664" s="5"/>
       <c r="B664" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C664" s="5"/>
       <c r="D664" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E664" s="3"/>
       <c r="F664" s="5"/>
@@ -15515,11 +15515,11 @@
     <row r="665" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A665" s="5"/>
       <c r="B665" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C665" s="5"/>
       <c r="D665" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E665" s="3"/>
       <c r="F665" s="5"/>
@@ -15533,11 +15533,11 @@
     <row r="666" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A666" s="5"/>
       <c r="B666" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C666" s="5"/>
       <c r="D666" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E666" s="3"/>
       <c r="F666" s="5"/>
@@ -15551,11 +15551,11 @@
     <row r="667" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A667" s="5"/>
       <c r="B667" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C667" s="5"/>
       <c r="D667" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E667" s="3"/>
       <c r="F667" s="5"/>
@@ -15569,11 +15569,11 @@
     <row r="668" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A668" s="5"/>
       <c r="B668" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C668" s="5"/>
       <c r="D668" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E668" s="3"/>
       <c r="F668" s="5"/>
@@ -15587,11 +15587,11 @@
     <row r="669" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A669" s="5"/>
       <c r="B669" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C669" s="5"/>
       <c r="D669" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E669" s="3"/>
       <c r="F669" s="5"/>
@@ -15605,11 +15605,11 @@
     <row r="670" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A670" s="5"/>
       <c r="B670" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C670" s="5"/>
       <c r="D670" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E670" s="3"/>
       <c r="F670" s="5"/>
@@ -15623,11 +15623,11 @@
     <row r="671" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A671" s="5"/>
       <c r="B671" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C671" s="5"/>
       <c r="D671" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E671" s="3"/>
       <c r="F671" s="5"/>
@@ -15641,11 +15641,11 @@
     <row r="672" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A672" s="5"/>
       <c r="B672" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C672" s="5"/>
       <c r="D672" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E672" s="3"/>
       <c r="F672" s="5"/>
@@ -15659,11 +15659,11 @@
     <row r="673" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A673" s="5"/>
       <c r="B673" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C673" s="5"/>
       <c r="D673" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E673" s="3"/>
       <c r="F673" s="5"/>
@@ -15677,11 +15677,11 @@
     <row r="674" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A674" s="5"/>
       <c r="B674" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C674" s="5"/>
       <c r="D674" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E674" s="3"/>
       <c r="F674" s="5"/>
@@ -15695,11 +15695,11 @@
     <row r="675" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A675" s="5"/>
       <c r="B675" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C675" s="5"/>
       <c r="D675" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E675" s="3"/>
       <c r="F675" s="5"/>
@@ -15713,11 +15713,11 @@
     <row r="676" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A676" s="5"/>
       <c r="B676" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C676" s="5"/>
       <c r="D676" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E676" s="3"/>
       <c r="F676" s="5"/>
@@ -15731,11 +15731,11 @@
     <row r="677" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A677" s="5"/>
       <c r="B677" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C677" s="5"/>
       <c r="D677" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E677" s="3"/>
       <c r="F677" s="5"/>
@@ -15749,11 +15749,11 @@
     <row r="678" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A678" s="5"/>
       <c r="B678" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C678" s="5"/>
       <c r="D678" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E678" s="3"/>
       <c r="F678" s="5"/>
@@ -15767,11 +15767,11 @@
     <row r="679" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A679" s="5"/>
       <c r="B679" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C679" s="5"/>
       <c r="D679" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E679" s="3"/>
       <c r="F679" s="5"/>
@@ -15785,11 +15785,11 @@
     <row r="680" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A680" s="5"/>
       <c r="B680" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C680" s="5"/>
       <c r="D680" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E680" s="3"/>
       <c r="F680" s="5"/>
@@ -15803,11 +15803,11 @@
     <row r="681" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A681" s="5"/>
       <c r="B681" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C681" s="5"/>
       <c r="D681" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E681" s="3"/>
       <c r="F681" s="5"/>
@@ -15821,11 +15821,11 @@
     <row r="682" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A682" s="5"/>
       <c r="B682" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C682" s="5"/>
       <c r="D682" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E682" s="3"/>
       <c r="F682" s="5"/>
@@ -15839,11 +15839,11 @@
     <row r="683" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A683" s="5"/>
       <c r="B683" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C683" s="5"/>
       <c r="D683" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E683" s="3"/>
       <c r="F683" s="5"/>
@@ -15857,11 +15857,11 @@
     <row r="684" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A684" s="5"/>
       <c r="B684" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C684" s="5"/>
       <c r="D684" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E684" s="3"/>
       <c r="F684" s="5"/>
@@ -15875,11 +15875,11 @@
     <row r="685" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A685" s="5"/>
       <c r="B685" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C685" s="5"/>
       <c r="D685" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E685" s="3"/>
       <c r="F685" s="5"/>
@@ -15893,11 +15893,11 @@
     <row r="686" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A686" s="5"/>
       <c r="B686" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C686" s="5"/>
       <c r="D686" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E686" s="3"/>
       <c r="F686" s="5"/>
@@ -15911,11 +15911,11 @@
     <row r="687" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A687" s="5"/>
       <c r="B687" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C687" s="5"/>
       <c r="D687" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E687" s="3"/>
       <c r="F687" s="5"/>
@@ -15929,11 +15929,11 @@
     <row r="688" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A688" s="5"/>
       <c r="B688" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C688" s="5"/>
       <c r="D688" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E688" s="3"/>
       <c r="F688" s="5"/>
@@ -15947,11 +15947,11 @@
     <row r="689" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A689" s="5"/>
       <c r="B689" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C689" s="5"/>
       <c r="D689" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E689" s="3"/>
       <c r="F689" s="5"/>
@@ -15965,11 +15965,11 @@
     <row r="690" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A690" s="5"/>
       <c r="B690" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C690" s="5"/>
       <c r="D690" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E690" s="3"/>
       <c r="F690" s="5"/>
@@ -15983,11 +15983,11 @@
     <row r="691" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A691" s="5"/>
       <c r="B691" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C691" s="5"/>
       <c r="D691" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E691" s="3"/>
       <c r="F691" s="5"/>
@@ -16001,11 +16001,11 @@
     <row r="692" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A692" s="5"/>
       <c r="B692" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C692" s="5"/>
       <c r="D692" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E692" s="3"/>
       <c r="F692" s="5"/>
@@ -16019,11 +16019,11 @@
     <row r="693" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A693" s="5"/>
       <c r="B693" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C693" s="5"/>
       <c r="D693" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E693" s="3"/>
       <c r="F693" s="5"/>
@@ -16037,11 +16037,11 @@
     <row r="694" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A694" s="5"/>
       <c r="B694" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C694" s="5"/>
       <c r="D694" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E694" s="3"/>
       <c r="F694" s="5"/>
@@ -16055,11 +16055,11 @@
     <row r="695" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A695" s="5"/>
       <c r="B695" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C695" s="5"/>
       <c r="D695" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E695" s="3"/>
       <c r="F695" s="5"/>
@@ -16073,11 +16073,11 @@
     <row r="696" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A696" s="5"/>
       <c r="B696" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C696" s="5"/>
       <c r="D696" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E696" s="3"/>
       <c r="F696" s="5"/>
@@ -16091,11 +16091,11 @@
     <row r="697" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A697" s="5"/>
       <c r="B697" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C697" s="5"/>
       <c r="D697" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E697" s="3"/>
       <c r="F697" s="5"/>
@@ -16109,11 +16109,11 @@
     <row r="698" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A698" s="5"/>
       <c r="B698" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C698" s="5"/>
       <c r="D698" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E698" s="3"/>
       <c r="F698" s="5"/>
@@ -16127,11 +16127,11 @@
     <row r="699" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A699" s="5"/>
       <c r="B699" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C699" s="5"/>
       <c r="D699" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E699" s="3"/>
       <c r="F699" s="5"/>
@@ -16145,11 +16145,11 @@
     <row r="700" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A700" s="5"/>
       <c r="B700" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C700" s="5"/>
       <c r="D700" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E700" s="3"/>
       <c r="F700" s="5"/>
@@ -16163,11 +16163,11 @@
     <row r="701" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A701" s="5"/>
       <c r="B701" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C701" s="5"/>
       <c r="D701" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E701" s="3"/>
       <c r="F701" s="5"/>
@@ -16181,11 +16181,11 @@
     <row r="702" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A702" s="5"/>
       <c r="B702" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C702" s="5"/>
       <c r="D702" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E702" s="3"/>
       <c r="F702" s="5"/>
@@ -16197,11 +16197,11 @@
     <row r="703" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A703" s="5"/>
       <c r="B703" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C703" s="5"/>
       <c r="D703" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E703" s="3"/>
       <c r="F703" s="5"/>
@@ -16215,11 +16215,11 @@
     <row r="704" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A704" s="5"/>
       <c r="B704" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C704" s="5"/>
       <c r="D704" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E704" s="3"/>
       <c r="F704" s="5"/>
@@ -16233,11 +16233,11 @@
     <row r="705" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A705" s="5"/>
       <c r="B705" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C705" s="5"/>
       <c r="D705" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E705" s="3"/>
       <c r="F705" s="5"/>
@@ -16251,11 +16251,11 @@
     <row r="706" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A706" s="5"/>
       <c r="B706" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C706" s="5"/>
       <c r="D706" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E706" s="3"/>
       <c r="F706" s="5"/>
@@ -16269,11 +16269,11 @@
     <row r="707" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A707" s="5"/>
       <c r="B707" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C707" s="5"/>
       <c r="D707" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E707" s="3"/>
       <c r="F707" s="5"/>
@@ -16287,11 +16287,11 @@
     <row r="708" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A708" s="5"/>
       <c r="B708" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C708" s="5"/>
       <c r="D708" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E708" s="3"/>
       <c r="F708" s="5"/>
@@ -16305,11 +16305,11 @@
     <row r="709" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A709" s="5"/>
       <c r="B709" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C709" s="5"/>
       <c r="D709" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E709" s="3"/>
       <c r="F709" s="5"/>
@@ -16323,11 +16323,11 @@
     <row r="710" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A710" s="5"/>
       <c r="B710" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C710" s="5"/>
       <c r="D710" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E710" s="3"/>
       <c r="F710" s="5"/>
@@ -16341,11 +16341,11 @@
     <row r="711" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A711" s="5"/>
       <c r="B711" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C711" s="5"/>
       <c r="D711" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E711" s="3"/>
       <c r="F711" s="5"/>
@@ -16359,11 +16359,11 @@
     <row r="712" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A712" s="5"/>
       <c r="B712" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C712" s="5"/>
       <c r="D712" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E712" s="3"/>
       <c r="F712" s="5"/>
@@ -16377,11 +16377,11 @@
     <row r="713" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A713" s="5"/>
       <c r="B713" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C713" s="5"/>
       <c r="D713" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E713" s="3"/>
       <c r="F713" s="5"/>
@@ -16395,11 +16395,11 @@
     <row r="714" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A714" s="5"/>
       <c r="B714" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C714" s="5"/>
       <c r="D714" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E714" s="3"/>
       <c r="F714" s="5"/>
@@ -16413,11 +16413,11 @@
     <row r="715" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A715" s="5"/>
       <c r="B715" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C715" s="5"/>
       <c r="D715" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E715" s="3"/>
       <c r="F715" s="5"/>
@@ -16431,11 +16431,11 @@
     <row r="716" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A716" s="5"/>
       <c r="B716" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C716" s="5"/>
       <c r="D716" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E716" s="3"/>
       <c r="F716" s="5"/>
@@ -16449,11 +16449,11 @@
     <row r="717" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A717" s="5"/>
       <c r="B717" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C717" s="5"/>
       <c r="D717" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E717" s="3"/>
       <c r="F717" s="5"/>
@@ -16467,11 +16467,11 @@
     <row r="718" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A718" s="5"/>
       <c r="B718" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C718" s="5"/>
       <c r="D718" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E718" s="3"/>
       <c r="F718" s="5"/>
@@ -16485,11 +16485,11 @@
     <row r="719" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A719" s="5"/>
       <c r="B719" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C719" s="5"/>
       <c r="D719" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E719" s="3"/>
       <c r="F719" s="5"/>
@@ -16503,11 +16503,11 @@
     <row r="720" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A720" s="5"/>
       <c r="B720" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C720" s="5"/>
       <c r="D720" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E720" s="3"/>
       <c r="F720" s="5"/>
@@ -16521,11 +16521,11 @@
     <row r="721" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A721" s="5"/>
       <c r="B721" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C721" s="5"/>
       <c r="D721" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E721" s="3"/>
       <c r="F721" s="5"/>
@@ -16539,11 +16539,11 @@
     <row r="722" spans="1:10" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A722" s="5"/>
       <c r="B722" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C722" s="5"/>
       <c r="D722" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E722" s="3"/>
       <c r="F722" s="5"/>
@@ -16569,7 +16569,7 @@
     <row r="724" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A724" s="5"/>
       <c r="B724" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C724" s="5"/>
       <c r="D724" s="5"/>
@@ -16585,7 +16585,7 @@
     <row r="725" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A725" s="5"/>
       <c r="B725" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C725" s="5"/>
       <c r="D725" s="5"/>
@@ -16598,10 +16598,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="726" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="726" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A726" s="5"/>
       <c r="B726" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C726" s="5"/>
       <c r="D726" s="5"/>
@@ -16614,10 +16614,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="727" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="727" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A727" s="5"/>
       <c r="B727" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C727" s="5"/>
       <c r="D727" s="5"/>
@@ -16630,10 +16630,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="728" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="728" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A728" s="5"/>
       <c r="B728" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C728" s="5"/>
       <c r="D728" s="5"/>
@@ -16649,7 +16649,7 @@
     <row r="729" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A729" s="5"/>
       <c r="B729" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C729" s="5"/>
       <c r="D729" s="5"/>
@@ -16662,10 +16662,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="730" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="730" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A730" s="5"/>
       <c r="B730" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C730" s="5"/>
       <c r="D730" s="5"/>
@@ -16681,7 +16681,7 @@
     <row r="731" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A731" s="5"/>
       <c r="B731" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C731" s="5"/>
       <c r="D731" s="5"/>
@@ -16697,7 +16697,7 @@
     <row r="732" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A732" s="5"/>
       <c r="B732" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C732" s="5"/>
       <c r="D732" s="5"/>
@@ -16713,7 +16713,7 @@
     <row r="733" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A733" s="5"/>
       <c r="B733" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C733" s="5"/>
       <c r="D733" s="5"/>
@@ -16729,7 +16729,7 @@
     <row r="734" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A734" s="5"/>
       <c r="B734" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C734" s="5"/>
       <c r="D734" s="5"/>
@@ -16745,7 +16745,7 @@
     <row r="735" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A735" s="5"/>
       <c r="B735" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C735" s="5"/>
       <c r="D735" s="5"/>
@@ -16758,10 +16758,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="736" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="736" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A736" s="5"/>
       <c r="B736" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C736" s="5"/>
       <c r="D736" s="5"/>
@@ -16786,10 +16786,10 @@
       <c r="I737" s="5"/>
       <c r="J737" s="5"/>
     </row>
-    <row r="738" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="738" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A738" s="5"/>
       <c r="B738" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C738" s="5"/>
       <c r="D738" s="5"/>
@@ -16802,10 +16802,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="739" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="739" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A739" s="5"/>
       <c r="B739" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C739" s="5"/>
       <c r="D739" s="5"/>
@@ -16818,10 +16818,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="740" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="740" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A740" s="5"/>
       <c r="B740" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C740" s="5"/>
       <c r="D740" s="5"/>
@@ -16834,10 +16834,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="741" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="741" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A741" s="5"/>
       <c r="B741" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C741" s="5"/>
       <c r="D741" s="5"/>
@@ -16850,10 +16850,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="742" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="742" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A742" s="5"/>
       <c r="B742" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C742" s="5"/>
       <c r="D742" s="5"/>
@@ -16869,7 +16869,7 @@
     <row r="743" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A743" s="5"/>
       <c r="B743" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C743" s="5"/>
       <c r="D743" s="5"/>
@@ -16885,7 +16885,7 @@
     <row r="744" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A744" s="5"/>
       <c r="B744" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C744" s="5"/>
       <c r="D744" s="5"/>
@@ -16901,7 +16901,7 @@
     <row r="745" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A745" s="5"/>
       <c r="B745" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C745" s="5"/>
       <c r="D745" s="5"/>
@@ -16917,7 +16917,7 @@
     <row r="746" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A746" s="5"/>
       <c r="B746" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C746" s="5"/>
       <c r="D746" s="5"/>
@@ -16930,10 +16930,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="747" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="747" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A747" s="5"/>
       <c r="B747" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C747" s="5"/>
       <c r="D747" s="5"/>
@@ -16949,7 +16949,7 @@
     <row r="748" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A748" s="5"/>
       <c r="B748" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C748" s="5"/>
       <c r="D748" s="5"/>
@@ -16965,7 +16965,7 @@
     <row r="749" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A749" s="5"/>
       <c r="B749" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C749" s="5"/>
       <c r="D749" s="5"/>
@@ -16978,10 +16978,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="750" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="750" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A750" s="5"/>
       <c r="B750" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C750" s="5"/>
       <c r="D750" s="5"/>
@@ -16997,7 +16997,7 @@
     <row r="751" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A751" s="5"/>
       <c r="B751" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C751" s="5"/>
       <c r="D751" s="5"/>
@@ -17013,7 +17013,7 @@
     <row r="752" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A752" s="5"/>
       <c r="B752" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C752" s="5"/>
       <c r="D752" s="5"/>
@@ -17029,7 +17029,7 @@
     <row r="753" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A753" s="5"/>
       <c r="B753" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C753" s="5"/>
       <c r="D753" s="5"/>
@@ -17042,10 +17042,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="754" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="754" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A754" s="5"/>
       <c r="B754" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C754" s="5"/>
       <c r="D754" s="5"/>
@@ -17061,7 +17061,7 @@
     <row r="755" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A755" s="5"/>
       <c r="B755" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C755" s="5"/>
       <c r="D755" s="5"/>
@@ -17077,7 +17077,7 @@
     <row r="756" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A756" s="5"/>
       <c r="B756" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C756" s="5"/>
       <c r="D756" s="5"/>
@@ -17093,7 +17093,7 @@
     <row r="757" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A757" s="5"/>
       <c r="B757" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="C757" s="5"/>
       <c r="D757" s="5"/>
@@ -17106,10 +17106,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="758" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="758" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A758" s="5"/>
       <c r="B758" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C758" s="5"/>
       <c r="D758" s="5"/>
@@ -17122,10 +17122,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="759" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="759" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A759" s="5"/>
       <c r="B759" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C759" s="5"/>
       <c r="D759" s="5"/>
@@ -17138,10 +17138,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="760" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="760" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A760" s="5"/>
       <c r="B760" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C760" s="5"/>
       <c r="D760" s="5"/>
@@ -17154,10 +17154,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="761" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="761" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A761" s="5"/>
       <c r="B761" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C761" s="5"/>
       <c r="D761" s="5"/>
@@ -17170,10 +17170,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="762" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="762" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A762" s="5"/>
       <c r="B762" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C762" s="5"/>
       <c r="D762" s="5"/>
@@ -17186,10 +17186,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="763" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="763" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A763" s="5"/>
       <c r="B763" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C763" s="5"/>
       <c r="D763" s="5"/>
@@ -17202,10 +17202,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="764" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="764" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A764" s="5"/>
       <c r="B764" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C764" s="5"/>
       <c r="D764" s="5"/>
@@ -17218,10 +17218,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="765" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="765" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A765" s="5"/>
       <c r="B765" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C765" s="5"/>
       <c r="D765" s="5"/>
@@ -17234,10 +17234,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="766" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="766" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A766" s="5"/>
       <c r="B766" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C766" s="5"/>
       <c r="D766" s="5"/>
@@ -17253,7 +17253,7 @@
     <row r="767" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A767" s="5"/>
       <c r="B767" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C767" s="5"/>
       <c r="D767" s="5"/>
@@ -17269,7 +17269,7 @@
     <row r="768" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A768" s="5"/>
       <c r="B768" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C768" s="5"/>
       <c r="D768" s="5"/>
@@ -17285,7 +17285,7 @@
     <row r="769" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A769" s="5"/>
       <c r="B769" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C769" s="5"/>
       <c r="D769" s="5"/>
@@ -17301,7 +17301,7 @@
     <row r="770" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A770" s="5"/>
       <c r="B770" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C770" s="5"/>
       <c r="D770" s="5"/>
@@ -17314,10 +17314,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="771" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="771" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A771" s="5"/>
       <c r="B771" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C771" s="5"/>
       <c r="D771" s="5"/>
@@ -17333,7 +17333,7 @@
     <row r="772" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A772" s="5"/>
       <c r="B772" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C772" s="5"/>
       <c r="D772" s="5"/>
@@ -17349,7 +17349,7 @@
     <row r="773" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A773" s="5"/>
       <c r="B773" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C773" s="5"/>
       <c r="D773" s="5"/>
@@ -17365,7 +17365,7 @@
     <row r="774" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A774" s="5"/>
       <c r="B774" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C774" s="5"/>
       <c r="D774" s="5"/>
@@ -17381,7 +17381,7 @@
     <row r="775" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A775" s="5"/>
       <c r="B775" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C775" s="5"/>
       <c r="D775" s="5"/>
@@ -17394,10 +17394,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="776" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="776" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A776" s="5"/>
       <c r="B776" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C776" s="5"/>
       <c r="D776" s="5"/>
@@ -17410,10 +17410,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="777" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="777" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A777" s="5"/>
       <c r="B777" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C777" s="5"/>
       <c r="D777" s="5"/>
@@ -17426,10 +17426,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="778" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="778" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A778" s="5"/>
       <c r="B778" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C778" s="5"/>
       <c r="D778" s="5"/>
@@ -17445,7 +17445,7 @@
     <row r="779" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A779" s="5"/>
       <c r="B779" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C779" s="5"/>
       <c r="D779" s="5"/>
@@ -17458,10 +17458,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="780" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="780" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A780" s="5"/>
       <c r="B780" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C780" s="5"/>
       <c r="D780" s="5"/>
@@ -17477,7 +17477,7 @@
     <row r="781" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A781" s="5"/>
       <c r="B781" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C781" s="5"/>
       <c r="D781" s="5"/>
@@ -17490,10 +17490,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="782" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="782" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A782" s="5"/>
       <c r="B782" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C782" s="5"/>
       <c r="D782" s="5"/>
@@ -17506,10 +17506,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="783" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="783" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A783" s="5"/>
       <c r="B783" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C783" s="5"/>
       <c r="D783" s="5"/>
@@ -17522,10 +17522,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="784" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="784" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A784" s="5"/>
       <c r="B784" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C784" s="5"/>
       <c r="D784" s="5"/>
@@ -17541,7 +17541,7 @@
     <row r="785" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A785" s="5"/>
       <c r="B785" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C785" s="5"/>
       <c r="D785" s="5"/>
@@ -17554,10 +17554,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="786" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="786" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A786" s="5"/>
       <c r="B786" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C786" s="5"/>
       <c r="D786" s="5"/>
@@ -17570,10 +17570,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="787" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="787" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A787" s="5"/>
       <c r="B787" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C787" s="5"/>
       <c r="D787" s="5"/>
@@ -17589,7 +17589,7 @@
     <row r="788" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A788" s="5"/>
       <c r="B788" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C788" s="5"/>
       <c r="D788" s="5"/>
@@ -17602,10 +17602,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="789" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="789" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A789" s="5"/>
       <c r="B789" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C789" s="5"/>
       <c r="D789" s="5"/>
@@ -17618,10 +17618,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="790" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="790" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A790" s="5"/>
       <c r="B790" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C790" s="5"/>
       <c r="D790" s="5"/>
@@ -17646,10 +17646,10 @@
       <c r="I791" s="5"/>
       <c r="J791" s="5"/>
     </row>
-    <row r="792" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="792" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A792" s="5"/>
       <c r="B792" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C792" s="5"/>
       <c r="D792" s="5"/>
@@ -17662,10 +17662,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="793" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="793" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A793" s="5"/>
       <c r="B793" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C793" s="5"/>
       <c r="D793" s="5"/>
@@ -17678,10 +17678,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="794" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="794" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A794" s="5"/>
       <c r="B794" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C794" s="5"/>
       <c r="D794" s="5"/>
@@ -17694,10 +17694,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="795" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="795" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A795" s="5"/>
       <c r="B795" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C795" s="5"/>
       <c r="D795" s="5"/>
@@ -17710,10 +17710,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="796" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="796" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A796" s="5"/>
       <c r="B796" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C796" s="5"/>
       <c r="D796" s="5"/>
@@ -17726,10 +17726,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="797" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="797" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A797" s="5"/>
       <c r="B797" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C797" s="5"/>
       <c r="D797" s="5"/>
@@ -17742,10 +17742,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="798" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="798" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A798" s="5"/>
       <c r="B798" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C798" s="5"/>
       <c r="D798" s="5"/>
@@ -17761,7 +17761,7 @@
     <row r="799" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A799" s="5"/>
       <c r="B799" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C799" s="5"/>
       <c r="D799" s="5"/>

</xml_diff>

<commit_message>
A bunch of bug fixes and add ons Bug fixes in constants, opminus, LegendreP-Q alternatives, CSV conversions. One bug remains,  just skip the space symbol but doesn't add multiplication symbol between 2 and a, which produces an error in Maple. Will fix that tomorrow.
</commit_message>
<xml_diff>
--- a/libs/ReferenceData/Maple.xlsx
+++ b/libs/ReferenceData/Maple.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maple2LaTeX" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="1172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="1176">
   <si>
     <t>Maple</t>
   </si>
@@ -2873,15 +2873,9 @@
     <t>\LamescdE{m}{2n+3}@{z}{k^2}</t>
   </si>
   <si>
-    <t>P($0, $1)</t>
-  </si>
-  <si>
     <t>\LegendrePoly{$0}@{$1}</t>
   </si>
   <si>
-    <t>This funcion needs an extra package. with(orthopoly)</t>
-  </si>
-  <si>
     <t>\LegendrePolys{n}@{x}</t>
   </si>
   <si>
@@ -3500,12 +3494,6 @@
     <t>KummerU($0, $1, $2)</t>
   </si>
   <si>
-    <t>This translation is only correct, when you previously set Maple's internal variable _EnvLegendreCut := 1..infinity. Use the "restart" command to clear the settings afterwards. More information can be found on Maple's website for LegendreP.</t>
-  </si>
-  <si>
-    <t>If you previously set Maple's internal variable _EnvLegendreCut := 1..infinity. You have to reset it. Use the "restart" command, since other functions such as evalf and simplify are also involved by changes in _EnvLegendreCut.</t>
-  </si>
-  <si>
     <t>\FerrersP{\nu}@{x}</t>
   </si>
   <si>
@@ -3518,9 +3506,6 @@
     <t>X1:\FerrersQX\FerrersQ[\mu]{\nu}@{x}</t>
   </si>
   <si>
-    <t>\FerrersP{$0}@{$1}</t>
-  </si>
-  <si>
     <t>\FerrersP[$1]{$0}@{$2}</t>
   </si>
   <si>
@@ -3540,13 +3525,40 @@
   </si>
   <si>
     <t>If your variable is real and you previously set _EnvLegendreCut := 1..infinity, the translation is not correct and you must use the alternative translation: \FerrersQ.</t>
+  </si>
+  <si>
+    <t>\FerrersP{$0}@{$1} || \LegendrePoly{$0}@{$1}</t>
+  </si>
+  <si>
+    <t>If you want to translate it, as the orthogonal polynomial, use the alternative \LegendrePoly. If your variable is real and you previously set _EnvLegendreCut := 1..infinity, the translation is not correct and you must use the alternative translation: \FerrersP.</t>
+  </si>
+  <si>
+    <t>Note that LegendreP is also the Legendre function.</t>
+  </si>
+  <si>
+    <t>LegendreP($0, 2*($1) - 1)</t>
+  </si>
+  <si>
+    <t>Note that LegendreP is also the Legendre function. This translation bases on DLMF 18.7.10.</t>
+  </si>
+  <si>
+    <t>This translation is only correct, when you previously set Maple's internal variable _EnvLegendreCut := 1..infinity. You have to invoke forget(evalf) and forget(simplify), otherwise these functions never noticed the changes of _EnvLegendreCut.</t>
+  </si>
+  <si>
+    <t>If you previously set Maple's internal variable _EnvLegendreCut := 1..infinity. You have to reset it to -1..1 and invoke forget(evalf) and forget(simplify) to notify Maple about the changes.</t>
+  </si>
+  <si>
+    <t>X2:LegendreQXLegendreQ($0,$1)/GAMMA($0+1)</t>
+  </si>
+  <si>
+    <t>X3:LegendreQXexp(-($1)*Pi*I)*LegendreQ($1,$0,$2)/GAMMA($0+$1+1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3636,6 +3648,11 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3718,7 +3735,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3868,6 +3885,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4187,8 +4207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z803"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="D407" sqref="D407"/>
+    <sheetView topLeftCell="A399" workbookViewId="0">
+      <selection activeCell="D403" sqref="D403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4215,7 +4235,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -4224,7 +4244,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -4965,7 +4985,7 @@
     <row r="46" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
@@ -4977,7 +4997,7 @@
     <row r="47" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
@@ -5874,10 +5894,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="C100" s="5">
         <v>2</v>
@@ -5887,15 +5907,15 @@
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
       <c r="H100" s="48" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="C101" s="5">
         <v>2</v>
@@ -5905,12 +5925,12 @@
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
       <c r="H101" s="48" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -5919,7 +5939,7 @@
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
       <c r="H102" s="48" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
@@ -9083,7 +9103,7 @@
         <v>519</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="C323" s="5">
         <v>1</v>
@@ -9171,7 +9191,7 @@
         <v>531</v>
       </c>
       <c r="B329" s="29" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C329" s="5">
         <v>6</v>
@@ -10305,7 +10325,7 @@
     <row r="399" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A399" s="3"/>
       <c r="B399" s="36" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="C399" s="5"/>
       <c r="D399" s="5"/>
@@ -10317,7 +10337,7 @@
     <row r="400" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A400" s="3"/>
       <c r="B400" s="36" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="C400" s="5"/>
       <c r="D400" s="5"/>
@@ -10329,7 +10349,7 @@
     <row r="401" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A401" s="5"/>
       <c r="B401" s="36" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="C401" s="5"/>
       <c r="D401" s="5"/>
@@ -10341,7 +10361,7 @@
     <row r="402" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A402" s="5"/>
       <c r="B402" s="36" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="C402" s="5"/>
       <c r="D402" s="5"/>
@@ -10350,23 +10370,23 @@
       <c r="G402" s="5"/>
       <c r="H402" s="5"/>
     </row>
-    <row r="403" spans="1:8" ht="81" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:8" ht="121.5" x14ac:dyDescent="0.3">
       <c r="A403" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B403" s="3" t="s">
         <v>1120</v>
-      </c>
-      <c r="B403" s="3" t="s">
-        <v>1122</v>
       </c>
       <c r="C403" s="5">
         <v>2</v>
       </c>
       <c r="D403" s="3" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="E403" s="5"/>
       <c r="F403" s="5"/>
       <c r="G403" s="5" t="s">
-        <v>1164</v>
+        <v>1167</v>
       </c>
       <c r="H403" s="6" t="s">
         <v>659</v>
@@ -10374,21 +10394,21 @@
     </row>
     <row r="404" spans="1:8" ht="81" x14ac:dyDescent="0.3">
       <c r="A404" s="3" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C404" s="5">
         <v>3</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="E404" s="5"/>
       <c r="F404" s="5"/>
       <c r="G404" s="5" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="H404" s="6" t="s">
         <v>659</v>
@@ -10396,21 +10416,21 @@
     </row>
     <row r="405" spans="1:8" ht="81" x14ac:dyDescent="0.3">
       <c r="A405" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B405" s="3" t="s">
         <v>1121</v>
-      </c>
-      <c r="B405" s="3" t="s">
-        <v>1123</v>
       </c>
       <c r="C405" s="5">
         <v>2</v>
       </c>
       <c r="D405" s="3" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="E405" s="5"/>
       <c r="F405" s="5"/>
       <c r="G405" s="5" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="H405" s="6" t="s">
         <v>660</v>
@@ -10418,21 +10438,21 @@
     </row>
     <row r="406" spans="1:8" ht="81" x14ac:dyDescent="0.3">
       <c r="A406" s="3" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C406" s="5">
         <v>3</v>
       </c>
       <c r="D406" s="3" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="E406" s="5"/>
       <c r="F406" s="5"/>
       <c r="G406" s="5" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="H406" s="6" t="s">
         <v>660</v>
@@ -10441,7 +10461,7 @@
     <row r="407" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A407" s="5"/>
       <c r="B407" s="36" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C407" s="5"/>
       <c r="D407" s="5"/>
@@ -10453,7 +10473,7 @@
     <row r="408" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A408" s="5"/>
       <c r="B408" s="36" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C408" s="5"/>
       <c r="D408" s="5"/>
@@ -10465,7 +10485,7 @@
     <row r="409" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A409" s="5"/>
       <c r="B409" s="42" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="C409" s="5"/>
       <c r="D409" s="5"/>
@@ -10479,7 +10499,7 @@
     <row r="410" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A410" s="5"/>
       <c r="B410" s="42" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="C410" s="5"/>
       <c r="D410" s="5"/>
@@ -13601,16 +13621,12 @@
       <c r="H630" s="5"/>
     </row>
     <row r="631" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A631" s="17" t="s">
+      <c r="A631" s="49"/>
+      <c r="B631" s="3" t="s">
         <v>949</v>
       </c>
-      <c r="B631" s="3" t="s">
-        <v>950</v>
-      </c>
-      <c r="C631" s="5">
-        <v>2</v>
-      </c>
-      <c r="D631" s="17"/>
+      <c r="C631" s="5"/>
+      <c r="D631" s="49"/>
       <c r="E631" s="5"/>
       <c r="F631" s="5"/>
       <c r="G631" s="5"/>
@@ -13621,7 +13637,7 @@
     <row r="632" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A632" s="5"/>
       <c r="B632" s="3" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C632" s="5"/>
       <c r="D632" s="5"/>
@@ -13635,7 +13651,7 @@
     <row r="633" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A633" s="5"/>
       <c r="B633" s="3" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C633" s="5"/>
       <c r="D633" s="5"/>
@@ -13659,7 +13675,7 @@
     <row r="635" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A635" s="5"/>
       <c r="B635" s="3" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C635" s="5"/>
       <c r="D635" s="5"/>
@@ -13673,7 +13689,7 @@
     <row r="636" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A636" s="5"/>
       <c r="B636" s="3" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C636" s="5"/>
       <c r="D636" s="5"/>
@@ -13687,7 +13703,7 @@
     <row r="637" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A637" s="5"/>
       <c r="B637" s="3" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C637" s="5"/>
       <c r="D637" s="5"/>
@@ -13701,7 +13717,7 @@
     <row r="638" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A638" s="5"/>
       <c r="B638" s="3" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C638" s="5"/>
       <c r="D638" s="5"/>
@@ -13725,7 +13741,7 @@
     <row r="640" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A640" s="5"/>
       <c r="B640" s="3" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C640" s="5"/>
       <c r="D640" s="5"/>
@@ -13749,7 +13765,7 @@
     <row r="642" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A642" s="5"/>
       <c r="B642" s="3" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C642" s="5"/>
       <c r="D642" s="5"/>
@@ -13773,7 +13789,7 @@
     <row r="644" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A644" s="5"/>
       <c r="B644" s="3" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C644" s="5"/>
       <c r="D644" s="5"/>
@@ -13787,7 +13803,7 @@
     <row r="645" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A645" s="5"/>
       <c r="B645" s="3" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="C645" s="5"/>
       <c r="D645" s="5"/>
@@ -13811,7 +13827,7 @@
     <row r="647" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A647" s="5"/>
       <c r="B647" s="3" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C647" s="5"/>
       <c r="D647" s="5"/>
@@ -13825,7 +13841,7 @@
     <row r="648" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A648" s="5"/>
       <c r="B648" s="3" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="C648" s="5"/>
       <c r="D648" s="5"/>
@@ -13849,7 +13865,7 @@
     <row r="650" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A650" s="5"/>
       <c r="B650" s="3" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C650" s="5"/>
       <c r="D650" s="5"/>
@@ -13863,7 +13879,7 @@
     <row r="651" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A651" s="5"/>
       <c r="B651" s="3" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C651" s="5"/>
       <c r="D651" s="5"/>
@@ -13887,7 +13903,7 @@
     <row r="653" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A653" s="5"/>
       <c r="B653" s="3" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C653" s="5"/>
       <c r="D653" s="5"/>
@@ -13941,7 +13957,7 @@
     <row r="658" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A658" s="5"/>
       <c r="B658" s="3" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C658" s="5"/>
       <c r="D658" s="3"/>
@@ -13955,7 +13971,7 @@
     <row r="659" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A659" s="5"/>
       <c r="B659" s="3" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C659" s="5"/>
       <c r="D659" s="3"/>
@@ -13969,7 +13985,7 @@
     <row r="660" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A660" s="5"/>
       <c r="B660" s="3" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C660" s="5"/>
       <c r="D660" s="3"/>
@@ -13983,7 +13999,7 @@
     <row r="661" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A661" s="5"/>
       <c r="B661" s="3" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C661" s="5"/>
       <c r="D661" s="3"/>
@@ -13997,7 +14013,7 @@
     <row r="662" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A662" s="5"/>
       <c r="B662" s="3" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C662" s="5"/>
       <c r="D662" s="3"/>
@@ -14011,7 +14027,7 @@
     <row r="663" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A663" s="5"/>
       <c r="B663" s="3" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C663" s="5"/>
       <c r="D663" s="3"/>
@@ -14025,7 +14041,7 @@
     <row r="664" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A664" s="5"/>
       <c r="B664" s="3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C664" s="5"/>
       <c r="D664" s="3"/>
@@ -14039,7 +14055,7 @@
     <row r="665" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A665" s="5"/>
       <c r="B665" s="3" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C665" s="5"/>
       <c r="D665" s="3"/>
@@ -14053,7 +14069,7 @@
     <row r="666" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A666" s="5"/>
       <c r="B666" s="3" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C666" s="5"/>
       <c r="D666" s="3"/>
@@ -14067,7 +14083,7 @@
     <row r="667" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A667" s="5"/>
       <c r="B667" s="3" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C667" s="5"/>
       <c r="D667" s="3"/>
@@ -14081,7 +14097,7 @@
     <row r="668" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A668" s="5"/>
       <c r="B668" s="3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C668" s="5"/>
       <c r="D668" s="3"/>
@@ -14095,7 +14111,7 @@
     <row r="669" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A669" s="5"/>
       <c r="B669" s="3" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C669" s="5"/>
       <c r="D669" s="3"/>
@@ -14109,7 +14125,7 @@
     <row r="670" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A670" s="5"/>
       <c r="B670" s="3" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C670" s="5"/>
       <c r="D670" s="3"/>
@@ -14123,7 +14139,7 @@
     <row r="671" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A671" s="5"/>
       <c r="B671" s="3" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C671" s="5"/>
       <c r="D671" s="3"/>
@@ -14137,7 +14153,7 @@
     <row r="672" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A672" s="5"/>
       <c r="B672" s="3" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C672" s="5"/>
       <c r="D672" s="3"/>
@@ -14151,7 +14167,7 @@
     <row r="673" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A673" s="5"/>
       <c r="B673" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C673" s="5"/>
       <c r="D673" s="3"/>
@@ -14179,7 +14195,7 @@
     <row r="675" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A675" s="5"/>
       <c r="B675" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C675" s="5"/>
       <c r="D675" s="3"/>
@@ -14193,7 +14209,7 @@
     <row r="676" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A676" s="5"/>
       <c r="B676" s="3" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C676" s="5"/>
       <c r="D676" s="3"/>
@@ -14207,7 +14223,7 @@
     <row r="677" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A677" s="5"/>
       <c r="B677" s="3" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C677" s="5"/>
       <c r="D677" s="3"/>
@@ -14221,7 +14237,7 @@
     <row r="678" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A678" s="5"/>
       <c r="B678" s="3" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C678" s="5"/>
       <c r="D678" s="3"/>
@@ -14235,7 +14251,7 @@
     <row r="679" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A679" s="5"/>
       <c r="B679" s="3" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C679" s="5"/>
       <c r="D679" s="3"/>
@@ -14249,7 +14265,7 @@
     <row r="680" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A680" s="5"/>
       <c r="B680" s="3" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C680" s="5"/>
       <c r="D680" s="3"/>
@@ -14263,7 +14279,7 @@
     <row r="681" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A681" s="5"/>
       <c r="B681" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C681" s="5"/>
       <c r="D681" s="3"/>
@@ -14277,7 +14293,7 @@
     <row r="682" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A682" s="5"/>
       <c r="B682" s="3" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C682" s="5"/>
       <c r="D682" s="3"/>
@@ -14291,7 +14307,7 @@
     <row r="683" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A683" s="5"/>
       <c r="B683" s="3" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="C683" s="5"/>
       <c r="D683" s="3"/>
@@ -14305,7 +14321,7 @@
     <row r="684" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A684" s="5"/>
       <c r="B684" s="3" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="C684" s="5"/>
       <c r="D684" s="3"/>
@@ -14319,7 +14335,7 @@
     <row r="685" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A685" s="5"/>
       <c r="B685" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C685" s="5"/>
       <c r="D685" s="3"/>
@@ -14333,7 +14349,7 @@
     <row r="686" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A686" s="5"/>
       <c r="B686" s="3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C686" s="5"/>
       <c r="D686" s="3"/>
@@ -14347,7 +14363,7 @@
     <row r="687" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A687" s="5"/>
       <c r="B687" s="3" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C687" s="5"/>
       <c r="D687" s="3"/>
@@ -14361,7 +14377,7 @@
     <row r="688" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A688" s="5"/>
       <c r="B688" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C688" s="5"/>
       <c r="D688" s="3"/>
@@ -14375,7 +14391,7 @@
     <row r="689" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A689" s="5"/>
       <c r="B689" s="3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="C689" s="5"/>
       <c r="D689" s="3"/>
@@ -14389,7 +14405,7 @@
     <row r="690" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A690" s="5"/>
       <c r="B690" s="3" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C690" s="5"/>
       <c r="D690" s="3"/>
@@ -14403,7 +14419,7 @@
     <row r="691" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A691" s="5"/>
       <c r="B691" s="3" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C691" s="5"/>
       <c r="D691" s="3"/>
@@ -14417,7 +14433,7 @@
     <row r="692" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A692" s="5"/>
       <c r="B692" s="3" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="C692" s="5"/>
       <c r="D692" s="3"/>
@@ -14431,7 +14447,7 @@
     <row r="693" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A693" s="5"/>
       <c r="B693" s="3" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C693" s="5"/>
       <c r="D693" s="3"/>
@@ -14445,7 +14461,7 @@
     <row r="694" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A694" s="5"/>
       <c r="B694" s="3" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="C694" s="5"/>
       <c r="D694" s="3"/>
@@ -14459,7 +14475,7 @@
     <row r="695" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A695" s="5"/>
       <c r="B695" s="3" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C695" s="5"/>
       <c r="D695" s="3"/>
@@ -14473,7 +14489,7 @@
     <row r="696" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A696" s="5"/>
       <c r="B696" s="3" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C696" s="5"/>
       <c r="D696" s="3"/>
@@ -14487,7 +14503,7 @@
     <row r="697" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A697" s="5"/>
       <c r="B697" s="3" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C697" s="5"/>
       <c r="D697" s="3"/>
@@ -14501,7 +14517,7 @@
     <row r="698" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A698" s="5"/>
       <c r="B698" s="3" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C698" s="5"/>
       <c r="D698" s="3"/>
@@ -14515,7 +14531,7 @@
     <row r="699" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A699" s="5"/>
       <c r="B699" s="3" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="C699" s="5"/>
       <c r="D699" s="3"/>
@@ -14529,7 +14545,7 @@
     <row r="700" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A700" s="5"/>
       <c r="B700" s="3" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C700" s="5"/>
       <c r="D700" s="3"/>
@@ -14543,7 +14559,7 @@
     <row r="701" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A701" s="5"/>
       <c r="B701" s="3" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="C701" s="5"/>
       <c r="D701" s="3"/>
@@ -14557,7 +14573,7 @@
     <row r="702" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A702" s="5"/>
       <c r="B702" s="3" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C702" s="5"/>
       <c r="D702" s="3"/>
@@ -14571,7 +14587,7 @@
     <row r="703" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A703" s="5"/>
       <c r="B703" s="3" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="C703" s="5"/>
       <c r="D703" s="3"/>
@@ -14585,7 +14601,7 @@
     <row r="704" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A704" s="5"/>
       <c r="B704" s="3" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C704" s="5"/>
       <c r="D704" s="3"/>
@@ -14597,7 +14613,7 @@
     <row r="705" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A705" s="5"/>
       <c r="B705" s="3" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="C705" s="5"/>
       <c r="D705" s="3"/>
@@ -14611,7 +14627,7 @@
     <row r="706" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A706" s="5"/>
       <c r="B706" s="3" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="C706" s="5"/>
       <c r="D706" s="3"/>
@@ -14625,7 +14641,7 @@
     <row r="707" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A707" s="5"/>
       <c r="B707" s="3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C707" s="5"/>
       <c r="D707" s="3"/>
@@ -14639,7 +14655,7 @@
     <row r="708" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A708" s="5"/>
       <c r="B708" s="3" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="C708" s="5"/>
       <c r="D708" s="3"/>
@@ -14653,7 +14669,7 @@
     <row r="709" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A709" s="5"/>
       <c r="B709" s="3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C709" s="5"/>
       <c r="D709" s="3"/>
@@ -14667,7 +14683,7 @@
     <row r="710" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A710" s="5"/>
       <c r="B710" s="3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="C710" s="5"/>
       <c r="D710" s="3"/>
@@ -14681,7 +14697,7 @@
     <row r="711" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A711" s="5"/>
       <c r="B711" s="3" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="C711" s="5"/>
       <c r="D711" s="3"/>
@@ -14695,7 +14711,7 @@
     <row r="712" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A712" s="5"/>
       <c r="B712" s="3" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C712" s="5"/>
       <c r="D712" s="3"/>
@@ -14709,7 +14725,7 @@
     <row r="713" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A713" s="5"/>
       <c r="B713" s="3" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="C713" s="5"/>
       <c r="D713" s="3"/>
@@ -14723,7 +14739,7 @@
     <row r="714" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A714" s="5"/>
       <c r="B714" s="3" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C714" s="5"/>
       <c r="D714" s="3"/>
@@ -14737,7 +14753,7 @@
     <row r="715" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A715" s="5"/>
       <c r="B715" s="3" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="C715" s="5"/>
       <c r="D715" s="3"/>
@@ -14751,7 +14767,7 @@
     <row r="716" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A716" s="5"/>
       <c r="B716" s="3" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C716" s="5"/>
       <c r="D716" s="3"/>
@@ -14765,7 +14781,7 @@
     <row r="717" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A717" s="5"/>
       <c r="B717" s="3" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="C717" s="5"/>
       <c r="D717" s="3"/>
@@ -14779,7 +14795,7 @@
     <row r="718" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A718" s="5"/>
       <c r="B718" s="3" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C718" s="5"/>
       <c r="D718" s="3"/>
@@ -14793,7 +14809,7 @@
     <row r="719" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A719" s="5"/>
       <c r="B719" s="3" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="C719" s="5"/>
       <c r="D719" s="3"/>
@@ -14807,7 +14823,7 @@
     <row r="720" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A720" s="5"/>
       <c r="B720" s="3" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C720" s="5"/>
       <c r="D720" s="3"/>
@@ -14821,7 +14837,7 @@
     <row r="721" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A721" s="5"/>
       <c r="B721" s="3" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="C721" s="5"/>
       <c r="D721" s="3"/>
@@ -14835,7 +14851,7 @@
     <row r="722" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A722" s="5"/>
       <c r="B722" s="3" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C722" s="5"/>
       <c r="D722" s="3"/>
@@ -14849,7 +14865,7 @@
     <row r="723" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A723" s="5"/>
       <c r="B723" s="3" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C723" s="5"/>
       <c r="D723" s="3"/>
@@ -14863,7 +14879,7 @@
     <row r="724" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A724" s="5"/>
       <c r="B724" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C724" s="5"/>
       <c r="D724" s="3"/>
@@ -14887,7 +14903,7 @@
     <row r="726" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A726" s="5"/>
       <c r="B726" s="3" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C726" s="5"/>
       <c r="D726" s="5"/>
@@ -14901,7 +14917,7 @@
     <row r="727" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A727" s="5"/>
       <c r="B727" s="3" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C727" s="5"/>
       <c r="D727" s="5"/>
@@ -14915,7 +14931,7 @@
     <row r="728" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A728" s="5"/>
       <c r="B728" s="3" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C728" s="5"/>
       <c r="D728" s="5"/>
@@ -14929,7 +14945,7 @@
     <row r="729" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A729" s="5"/>
       <c r="B729" s="3" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C729" s="5"/>
       <c r="D729" s="5"/>
@@ -14943,7 +14959,7 @@
     <row r="730" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A730" s="5"/>
       <c r="B730" s="3" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C730" s="5"/>
       <c r="D730" s="5"/>
@@ -14957,7 +14973,7 @@
     <row r="731" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A731" s="5"/>
       <c r="B731" s="3" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C731" s="5"/>
       <c r="D731" s="5"/>
@@ -14971,7 +14987,7 @@
     <row r="732" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A732" s="5"/>
       <c r="B732" s="3" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="C732" s="5"/>
       <c r="D732" s="5"/>
@@ -14985,7 +15001,7 @@
     <row r="733" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A733" s="5"/>
       <c r="B733" s="3" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C733" s="5"/>
       <c r="D733" s="5"/>
@@ -14999,7 +15015,7 @@
     <row r="734" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A734" s="5"/>
       <c r="B734" s="3" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="C734" s="5"/>
       <c r="D734" s="5"/>
@@ -15013,7 +15029,7 @@
     <row r="735" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A735" s="5"/>
       <c r="B735" s="3" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C735" s="5"/>
       <c r="D735" s="5"/>
@@ -15027,7 +15043,7 @@
     <row r="736" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A736" s="5"/>
       <c r="B736" s="3" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="C736" s="5"/>
       <c r="D736" s="5"/>
@@ -15041,7 +15057,7 @@
     <row r="737" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A737" s="5"/>
       <c r="B737" s="3" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C737" s="5"/>
       <c r="D737" s="5"/>
@@ -15055,7 +15071,7 @@
     <row r="738" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A738" s="5"/>
       <c r="B738" s="3" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="C738" s="5"/>
       <c r="D738" s="5"/>
@@ -15079,7 +15095,7 @@
     <row r="740" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A740" s="5"/>
       <c r="B740" s="3" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="C740" s="5"/>
       <c r="D740" s="5"/>
@@ -15093,7 +15109,7 @@
     <row r="741" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A741" s="5"/>
       <c r="B741" s="3" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C741" s="5"/>
       <c r="D741" s="5"/>
@@ -15107,7 +15123,7 @@
     <row r="742" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A742" s="5"/>
       <c r="B742" s="3" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="C742" s="5"/>
       <c r="D742" s="5"/>
@@ -15121,7 +15137,7 @@
     <row r="743" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A743" s="5"/>
       <c r="B743" s="3" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="C743" s="5"/>
       <c r="D743" s="5"/>
@@ -15135,7 +15151,7 @@
     <row r="744" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A744" s="5"/>
       <c r="B744" s="3" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C744" s="5"/>
       <c r="D744" s="5"/>
@@ -15149,7 +15165,7 @@
     <row r="745" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A745" s="5"/>
       <c r="B745" s="3" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C745" s="5"/>
       <c r="D745" s="5"/>
@@ -15163,7 +15179,7 @@
     <row r="746" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A746" s="5"/>
       <c r="B746" s="3" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C746" s="5"/>
       <c r="D746" s="5"/>
@@ -15205,7 +15221,7 @@
     <row r="749" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A749" s="5"/>
       <c r="B749" s="3" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C749" s="5"/>
       <c r="D749" s="5"/>
@@ -15219,7 +15235,7 @@
     <row r="750" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A750" s="5"/>
       <c r="B750" s="3" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C750" s="5"/>
       <c r="D750" s="5"/>
@@ -15233,7 +15249,7 @@
     <row r="751" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A751" s="5"/>
       <c r="B751" s="3" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="C751" s="5"/>
       <c r="D751" s="5"/>
@@ -15247,7 +15263,7 @@
     <row r="752" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A752" s="5"/>
       <c r="B752" s="3" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C752" s="5"/>
       <c r="D752" s="5"/>
@@ -15261,7 +15277,7 @@
     <row r="753" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A753" s="5"/>
       <c r="B753" s="3" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="C753" s="5"/>
       <c r="D753" s="5"/>
@@ -15275,7 +15291,7 @@
     <row r="754" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A754" s="5"/>
       <c r="B754" s="3" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C754" s="5"/>
       <c r="D754" s="5"/>
@@ -15289,7 +15305,7 @@
     <row r="755" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A755" s="5"/>
       <c r="B755" s="3" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="C755" s="5"/>
       <c r="D755" s="5"/>
@@ -15303,7 +15319,7 @@
     <row r="756" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A756" s="5"/>
       <c r="B756" s="3" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C756" s="5"/>
       <c r="D756" s="5"/>
@@ -15317,7 +15333,7 @@
     <row r="757" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A757" s="5"/>
       <c r="B757" s="3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C757" s="5"/>
       <c r="D757" s="5"/>
@@ -15331,7 +15347,7 @@
     <row r="758" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A758" s="5"/>
       <c r="B758" s="3" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="C758" s="5"/>
       <c r="D758" s="5"/>
@@ -15345,7 +15361,7 @@
     <row r="759" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A759" s="5"/>
       <c r="B759" s="3" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="C759" s="5"/>
       <c r="D759" s="5"/>
@@ -15359,7 +15375,7 @@
     <row r="760" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A760" s="5"/>
       <c r="B760" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="C760" s="5"/>
       <c r="D760" s="5"/>
@@ -15373,7 +15389,7 @@
     <row r="761" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A761" s="5"/>
       <c r="B761" s="3" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="C761" s="5"/>
       <c r="D761" s="5"/>
@@ -15387,7 +15403,7 @@
     <row r="762" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A762" s="5"/>
       <c r="B762" s="3" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C762" s="5"/>
       <c r="D762" s="5"/>
@@ -15401,7 +15417,7 @@
     <row r="763" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A763" s="5"/>
       <c r="B763" s="3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="C763" s="5"/>
       <c r="D763" s="5"/>
@@ -15415,7 +15431,7 @@
     <row r="764" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A764" s="5"/>
       <c r="B764" s="3" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="C764" s="5"/>
       <c r="D764" s="5"/>
@@ -15429,7 +15445,7 @@
     <row r="765" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A765" s="5"/>
       <c r="B765" s="3" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="C765" s="5"/>
       <c r="D765" s="5"/>
@@ -15443,7 +15459,7 @@
     <row r="766" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A766" s="5"/>
       <c r="B766" s="3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="C766" s="5"/>
       <c r="D766" s="5"/>
@@ -15457,7 +15473,7 @@
     <row r="767" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A767" s="5"/>
       <c r="B767" s="3" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C767" s="5"/>
       <c r="D767" s="5"/>
@@ -15471,7 +15487,7 @@
     <row r="768" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A768" s="5"/>
       <c r="B768" s="3" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="C768" s="5"/>
       <c r="D768" s="5"/>
@@ -15485,7 +15501,7 @@
     <row r="769" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A769" s="5"/>
       <c r="B769" s="3" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C769" s="5"/>
       <c r="D769" s="5"/>
@@ -15499,7 +15515,7 @@
     <row r="770" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A770" s="5"/>
       <c r="B770" s="3" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="C770" s="5"/>
       <c r="D770" s="5"/>
@@ -15513,7 +15529,7 @@
     <row r="771" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A771" s="5"/>
       <c r="B771" s="3" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="C771" s="5"/>
       <c r="D771" s="5"/>
@@ -15527,7 +15543,7 @@
     <row r="772" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A772" s="5"/>
       <c r="B772" s="3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C772" s="5"/>
       <c r="D772" s="5"/>
@@ -15541,7 +15557,7 @@
     <row r="773" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A773" s="5"/>
       <c r="B773" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="C773" s="5"/>
       <c r="D773" s="5"/>
@@ -15555,7 +15571,7 @@
     <row r="774" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A774" s="5"/>
       <c r="B774" s="3" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="C774" s="5"/>
       <c r="D774" s="5"/>
@@ -15569,7 +15585,7 @@
     <row r="775" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A775" s="5"/>
       <c r="B775" s="3" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="C775" s="5"/>
       <c r="D775" s="5"/>
@@ -15583,7 +15599,7 @@
     <row r="776" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A776" s="5"/>
       <c r="B776" s="3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="C776" s="5"/>
       <c r="D776" s="5"/>
@@ -15597,7 +15613,7 @@
     <row r="777" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A777" s="5"/>
       <c r="B777" s="3" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C777" s="5"/>
       <c r="D777" s="5"/>
@@ -15611,7 +15627,7 @@
     <row r="778" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A778" s="5"/>
       <c r="B778" s="3" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="C778" s="5"/>
       <c r="D778" s="5"/>
@@ -15625,7 +15641,7 @@
     <row r="779" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A779" s="5"/>
       <c r="B779" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="C779" s="5"/>
       <c r="D779" s="5"/>
@@ -15639,7 +15655,7 @@
     <row r="780" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A780" s="5"/>
       <c r="B780" s="3" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C780" s="5"/>
       <c r="D780" s="5"/>
@@ -15653,7 +15669,7 @@
     <row r="781" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A781" s="5"/>
       <c r="B781" s="3" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C781" s="5"/>
       <c r="D781" s="5"/>
@@ -15667,7 +15683,7 @@
     <row r="782" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A782" s="5"/>
       <c r="B782" s="3" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C782" s="5"/>
       <c r="D782" s="5"/>
@@ -15681,7 +15697,7 @@
     <row r="783" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A783" s="5"/>
       <c r="B783" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="C783" s="5"/>
       <c r="D783" s="5"/>
@@ -15695,7 +15711,7 @@
     <row r="784" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A784" s="5"/>
       <c r="B784" s="3" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="C784" s="5"/>
       <c r="D784" s="5"/>
@@ -15709,7 +15725,7 @@
     <row r="785" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A785" s="5"/>
       <c r="B785" s="3" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="C785" s="5"/>
       <c r="D785" s="5"/>
@@ -15723,7 +15739,7 @@
     <row r="786" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A786" s="5"/>
       <c r="B786" s="3" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C786" s="5"/>
       <c r="D786" s="5"/>
@@ -15737,7 +15753,7 @@
     <row r="787" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A787" s="5"/>
       <c r="B787" s="3" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="C787" s="5"/>
       <c r="D787" s="5"/>
@@ -15751,7 +15767,7 @@
     <row r="788" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A788" s="5"/>
       <c r="B788" s="3" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C788" s="5"/>
       <c r="D788" s="5"/>
@@ -15765,7 +15781,7 @@
     <row r="789" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A789" s="5"/>
       <c r="B789" s="3" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="C789" s="5"/>
       <c r="D789" s="5"/>
@@ -15779,7 +15795,7 @@
     <row r="790" spans="1:8" ht="27" x14ac:dyDescent="0.3">
       <c r="A790" s="5"/>
       <c r="B790" s="3" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="C790" s="5"/>
       <c r="D790" s="5"/>
@@ -15793,7 +15809,7 @@
     <row r="791" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A791" s="5"/>
       <c r="B791" s="3" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C791" s="5"/>
       <c r="D791" s="5"/>
@@ -15807,7 +15823,7 @@
     <row r="792" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A792" s="5"/>
       <c r="B792" s="3" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C792" s="5"/>
       <c r="D792" s="5"/>
@@ -15831,7 +15847,7 @@
     <row r="794" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A794" s="5"/>
       <c r="B794" s="3" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="C794" s="5"/>
       <c r="D794" s="5"/>
@@ -15845,7 +15861,7 @@
     <row r="795" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A795" s="5"/>
       <c r="B795" s="3" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="C795" s="5"/>
       <c r="D795" s="5"/>
@@ -15859,7 +15875,7 @@
     <row r="796" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A796" s="5"/>
       <c r="B796" s="3" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="C796" s="5"/>
       <c r="D796" s="5"/>
@@ -15873,7 +15889,7 @@
     <row r="797" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A797" s="5"/>
       <c r="B797" s="3" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="C797" s="5"/>
       <c r="D797" s="5"/>
@@ -15887,7 +15903,7 @@
     <row r="798" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A798" s="5"/>
       <c r="B798" s="3" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="C798" s="5"/>
       <c r="D798" s="5"/>
@@ -15901,7 +15917,7 @@
     <row r="799" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A799" s="5"/>
       <c r="B799" s="3" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C799" s="5"/>
       <c r="D799" s="5"/>
@@ -15915,7 +15931,7 @@
     <row r="800" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A800" s="5"/>
       <c r="B800" s="3" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C800" s="5"/>
       <c r="D800" s="5"/>
@@ -15929,7 +15945,7 @@
     <row r="801" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A801" s="5"/>
       <c r="B801" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C801" s="5"/>
       <c r="D801" s="5"/>
@@ -16206,8 +16222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W799"/>
   <sheetViews>
-    <sheetView topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="B404" sqref="B404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16231,10 +16247,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
@@ -16493,7 +16509,7 @@
         <v>57</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
@@ -16744,7 +16760,7 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="37" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
@@ -16769,24 +16785,24 @@
     </row>
     <row r="46" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="3" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
@@ -16841,7 +16857,7 @@
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="37" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="13.5" x14ac:dyDescent="0.3">
@@ -16856,7 +16872,7 @@
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="37" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="52" spans="1:23" ht="13.5" x14ac:dyDescent="0.3">
@@ -16906,7 +16922,7 @@
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="37" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="56" spans="1:23" ht="13.5" x14ac:dyDescent="0.3">
@@ -17026,7 +17042,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="E64" s="3"/>
     </row>
@@ -17095,15 +17111,15 @@
         <v>1</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>172</v>
@@ -17239,7 +17255,7 @@
         <v>206</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="C83" s="5">
         <v>4</v>
@@ -17287,7 +17303,7 @@
         <v>215</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C89" s="5">
         <v>4</v>
@@ -17603,7 +17619,7 @@
     </row>
     <row r="122" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>257</v>
@@ -17634,7 +17650,7 @@
     </row>
     <row r="125" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>264</v>
@@ -17647,7 +17663,7 @@
     </row>
     <row r="126" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>267</v>
@@ -19785,7 +19801,7 @@
         <v>561</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="C339" s="5">
         <v>3</v>
@@ -19798,7 +19814,7 @@
         <v>564</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C340" s="5">
         <v>3</v>
@@ -20243,10 +20259,10 @@
     </row>
     <row r="376" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A376" s="3" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B376" s="32" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C376" s="5">
         <v>2</v>
@@ -20435,147 +20451,155 @@
       <c r="D395" s="5"/>
       <c r="E395" s="36"/>
     </row>
-    <row r="396" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:5" ht="108" x14ac:dyDescent="0.3">
       <c r="A396" s="36" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C396" s="5">
         <v>2</v>
       </c>
       <c r="D396" s="36" t="s">
-        <v>1158</v>
+        <v>1172</v>
       </c>
       <c r="E396" s="36"/>
     </row>
-    <row r="397" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:5" ht="108" x14ac:dyDescent="0.3">
       <c r="A397" s="36" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="C397" s="5">
         <v>3</v>
       </c>
       <c r="D397" s="36" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E397" s="36"/>
+    </row>
+    <row r="398" spans="1:5" ht="108" x14ac:dyDescent="0.3">
+      <c r="A398" s="36" t="s">
         <v>1158</v>
       </c>
-      <c r="E397" s="36"/>
-    </row>
-    <row r="398" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
-      <c r="A398" s="36" t="s">
-        <v>1162</v>
-      </c>
       <c r="B398" s="3" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="C398" s="5">
         <v>2</v>
       </c>
       <c r="D398" s="36" t="s">
-        <v>1158</v>
+        <v>1172</v>
       </c>
       <c r="E398" s="36"/>
     </row>
-    <row r="399" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:5" ht="108" x14ac:dyDescent="0.3">
       <c r="A399" s="36" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C399" s="5">
         <v>3</v>
       </c>
       <c r="D399" s="36" t="s">
-        <v>1158</v>
+        <v>1172</v>
       </c>
       <c r="E399" s="36"/>
     </row>
-    <row r="400" spans="1:5" ht="108" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A400" s="3" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C400" s="5">
         <v>2</v>
       </c>
       <c r="D400" s="36" t="s">
-        <v>1159</v>
+        <v>1173</v>
       </c>
       <c r="E400" s="36"/>
     </row>
-    <row r="401" spans="1:5" ht="108" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A401" s="3" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="C401" s="5">
         <v>3</v>
       </c>
       <c r="D401" s="36" t="s">
-        <v>1159</v>
+        <v>1173</v>
       </c>
       <c r="E401" s="3"/>
     </row>
-    <row r="402" spans="1:5" ht="108" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A402" s="3" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="C402" s="5">
         <v>2</v>
       </c>
       <c r="D402" s="36" t="s">
-        <v>1159</v>
+        <v>1173</v>
       </c>
       <c r="E402" s="36"/>
     </row>
-    <row r="403" spans="1:5" ht="108" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A403" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C403" s="5">
         <v>3</v>
       </c>
       <c r="D403" s="36" t="s">
-        <v>1159</v>
+        <v>1173</v>
       </c>
       <c r="E403" s="36"/>
     </row>
     <row r="404" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A404" s="36" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B404" s="5"/>
-      <c r="C404" s="5"/>
+        <v>1122</v>
+      </c>
+      <c r="B404" s="5" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C404" s="5">
+        <v>2</v>
+      </c>
       <c r="D404" s="5"/>
       <c r="E404" s="36"/>
     </row>
-    <row r="405" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:5" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A405" s="36" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B405" s="5"/>
-      <c r="C405" s="5"/>
+        <v>1125</v>
+      </c>
+      <c r="B405" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C405" s="5">
+        <v>3</v>
+      </c>
       <c r="D405" s="5"/>
       <c r="E405" s="36"/>
     </row>
     <row r="406" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A406" s="42" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="B406" s="5"/>
       <c r="C406" s="5"/>
@@ -20584,7 +20608,7 @@
     </row>
     <row r="407" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A407" s="42" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="B407" s="5"/>
       <c r="C407" s="5"/>
@@ -20600,7 +20624,7 @@
     </row>
     <row r="409" spans="1:5" ht="54" x14ac:dyDescent="0.3">
       <c r="A409" s="16" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="B409" s="16" t="s">
         <v>661</v>
@@ -20612,12 +20636,12 @@
         <v>663</v>
       </c>
       <c r="E409" s="37" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="410" spans="1:5" ht="54" x14ac:dyDescent="0.3">
       <c r="A410" s="16" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="B410" s="16" t="s">
         <v>665</v>
@@ -20632,7 +20656,7 @@
     </row>
     <row r="411" spans="1:5" ht="54" x14ac:dyDescent="0.3">
       <c r="A411" s="16" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="B411" s="16" t="s">
         <v>668</v>
@@ -20666,7 +20690,7 @@
       </c>
       <c r="D413" s="3"/>
       <c r="E413" s="37" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="414" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
@@ -22068,7 +22092,7 @@
         <v>868</v>
       </c>
       <c r="B554" s="3" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C554" s="5">
         <v>2</v>
@@ -22750,38 +22774,44 @@
     </row>
     <row r="627" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A627" s="5"/>
-      <c r="B627" s="5"/>
-      <c r="C627" s="5"/>
-      <c r="D627" s="5"/>
-      <c r="E627" s="36"/>
+      <c r="B627" s="51"/>
+      <c r="C627" s="51"/>
+      <c r="D627" s="51"/>
+      <c r="E627" s="42"/>
     </row>
     <row r="628" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A628" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="B628" s="42" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C628" s="51">
+        <v>2</v>
+      </c>
+      <c r="D628" s="42" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E628" s="42"/>
+    </row>
+    <row r="629" spans="1:5" ht="54" x14ac:dyDescent="0.3">
+      <c r="A629" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="B628" s="49"/>
-      <c r="C628" s="5">
+      <c r="B629" s="42" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C629" s="51">
         <v>2</v>
       </c>
-      <c r="D628" s="17" t="s">
-        <v>951</v>
-      </c>
-      <c r="E628" s="17" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="629" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A629" s="3" t="s">
-        <v>952</v>
-      </c>
-      <c r="B629" s="5"/>
-      <c r="C629" s="5"/>
-      <c r="D629" s="5"/>
-      <c r="E629" s="36"/>
+      <c r="D629" s="42" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E629" s="42"/>
     </row>
     <row r="630" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A630" s="3" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B630" s="5"/>
       <c r="C630" s="5"/>
@@ -22797,7 +22827,7 @@
     </row>
     <row r="632" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A632" s="3" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B632" s="5"/>
       <c r="C632" s="5"/>
@@ -22806,7 +22836,7 @@
     </row>
     <row r="633" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A633" s="3" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B633" s="5"/>
       <c r="C633" s="5"/>
@@ -22815,7 +22845,7 @@
     </row>
     <row r="634" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A634" s="3" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B634" s="5"/>
       <c r="C634" s="5"/>
@@ -22824,7 +22854,7 @@
     </row>
     <row r="635" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A635" s="3" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B635" s="5"/>
       <c r="C635" s="5"/>
@@ -22840,7 +22870,7 @@
     </row>
     <row r="637" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A637" s="3" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B637" s="5"/>
       <c r="C637" s="5"/>
@@ -22856,7 +22886,7 @@
     </row>
     <row r="639" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A639" s="3" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B639" s="5"/>
       <c r="C639" s="5"/>
@@ -22872,7 +22902,7 @@
     </row>
     <row r="641" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A641" s="3" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="B641" s="5"/>
       <c r="C641" s="5"/>
@@ -22881,7 +22911,7 @@
     </row>
     <row r="642" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A642" s="3" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B642" s="5"/>
       <c r="C642" s="5"/>
@@ -22897,7 +22927,7 @@
     </row>
     <row r="644" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A644" s="3" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="B644" s="5"/>
       <c r="C644" s="5"/>
@@ -22906,7 +22936,7 @@
     </row>
     <row r="645" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A645" s="3" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B645" s="5"/>
       <c r="C645" s="5"/>
@@ -22922,7 +22952,7 @@
     </row>
     <row r="647" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A647" s="3" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="B647" s="5"/>
       <c r="C647" s="5"/>
@@ -22931,7 +22961,7 @@
     </row>
     <row r="648" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A648" s="3" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B648" s="5"/>
       <c r="C648" s="5"/>
@@ -22947,7 +22977,7 @@
     </row>
     <row r="650" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A650" s="3" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B650" s="5"/>
       <c r="C650" s="5"/>
@@ -22993,177 +23023,177 @@
     </row>
     <row r="655" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A655" s="3" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B655" s="5"/>
       <c r="C655" s="5"/>
       <c r="D655" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E655" s="36"/>
     </row>
     <row r="656" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A656" s="3" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B656" s="5"/>
       <c r="C656" s="5"/>
       <c r="D656" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E656" s="36"/>
     </row>
     <row r="657" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A657" s="3" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B657" s="5"/>
       <c r="C657" s="5"/>
       <c r="D657" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E657" s="36"/>
     </row>
     <row r="658" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A658" s="3" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B658" s="5"/>
       <c r="C658" s="5"/>
       <c r="D658" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E658" s="36"/>
     </row>
     <row r="659" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A659" s="3" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B659" s="5"/>
       <c r="C659" s="5"/>
       <c r="D659" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E659" s="36"/>
     </row>
     <row r="660" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A660" s="3" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B660" s="5"/>
       <c r="C660" s="5"/>
       <c r="D660" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E660" s="36"/>
     </row>
     <row r="661" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A661" s="3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B661" s="5"/>
       <c r="C661" s="5"/>
       <c r="D661" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E661" s="36"/>
     </row>
     <row r="662" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A662" s="3" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B662" s="5"/>
       <c r="C662" s="5"/>
       <c r="D662" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E662" s="36"/>
     </row>
     <row r="663" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A663" s="3" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B663" s="5"/>
       <c r="C663" s="5"/>
       <c r="D663" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E663" s="36"/>
     </row>
     <row r="664" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A664" s="3" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B664" s="5"/>
       <c r="C664" s="5"/>
       <c r="D664" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E664" s="36"/>
     </row>
     <row r="665" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A665" s="3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B665" s="5"/>
       <c r="C665" s="5"/>
       <c r="D665" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E665" s="36"/>
     </row>
     <row r="666" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A666" s="3" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B666" s="5"/>
       <c r="C666" s="5"/>
       <c r="D666" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E666" s="36"/>
     </row>
     <row r="667" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A667" s="3" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B667" s="5"/>
       <c r="C667" s="5"/>
       <c r="D667" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E667" s="36"/>
     </row>
     <row r="668" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A668" s="3" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B668" s="5"/>
       <c r="C668" s="5"/>
       <c r="D668" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E668" s="36"/>
     </row>
     <row r="669" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A669" s="3" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B669" s="5"/>
       <c r="C669" s="5"/>
       <c r="D669" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E669" s="36"/>
     </row>
     <row r="670" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A670" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="B670" s="5"/>
       <c r="C670" s="5"/>
       <c r="D670" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E670" s="36"/>
     </row>
@@ -23174,557 +23204,557 @@
       <c r="B671" s="5"/>
       <c r="C671" s="5"/>
       <c r="D671" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E671" s="36"/>
     </row>
     <row r="672" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A672" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B672" s="5"/>
       <c r="C672" s="5"/>
       <c r="D672" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E672" s="36"/>
     </row>
     <row r="673" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A673" s="3" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B673" s="5"/>
       <c r="C673" s="5"/>
       <c r="D673" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E673" s="36"/>
     </row>
     <row r="674" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A674" s="3" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B674" s="5"/>
       <c r="C674" s="5"/>
       <c r="D674" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E674" s="36"/>
     </row>
     <row r="675" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A675" s="3" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B675" s="5"/>
       <c r="C675" s="5"/>
       <c r="D675" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E675" s="36"/>
     </row>
     <row r="676" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A676" s="3" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B676" s="5"/>
       <c r="C676" s="5"/>
       <c r="D676" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E676" s="36"/>
     </row>
     <row r="677" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A677" s="3" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B677" s="5"/>
       <c r="C677" s="5"/>
       <c r="D677" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E677" s="36"/>
     </row>
     <row r="678" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A678" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B678" s="5"/>
       <c r="C678" s="5"/>
       <c r="D678" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E678" s="36"/>
     </row>
     <row r="679" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A679" s="3" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B679" s="5"/>
       <c r="C679" s="5"/>
       <c r="D679" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E679" s="36"/>
     </row>
     <row r="680" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A680" s="3" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B680" s="5"/>
       <c r="C680" s="5"/>
       <c r="D680" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E680" s="36"/>
     </row>
     <row r="681" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A681" s="3" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B681" s="5"/>
       <c r="C681" s="5"/>
       <c r="D681" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E681" s="36"/>
     </row>
     <row r="682" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A682" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B682" s="5"/>
       <c r="C682" s="5"/>
       <c r="D682" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E682" s="36"/>
     </row>
     <row r="683" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A683" s="3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B683" s="5"/>
       <c r="C683" s="5"/>
       <c r="D683" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E683" s="36"/>
     </row>
     <row r="684" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A684" s="3" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B684" s="5"/>
       <c r="C684" s="5"/>
       <c r="D684" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E684" s="36"/>
     </row>
     <row r="685" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A685" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B685" s="5"/>
       <c r="C685" s="5"/>
       <c r="D685" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E685" s="36"/>
     </row>
     <row r="686" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A686" s="3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B686" s="5"/>
       <c r="C686" s="5"/>
       <c r="D686" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E686" s="36"/>
     </row>
     <row r="687" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A687" s="3" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B687" s="5"/>
       <c r="C687" s="5"/>
       <c r="D687" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E687" s="36"/>
     </row>
     <row r="688" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A688" s="3" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B688" s="5"/>
       <c r="C688" s="5"/>
       <c r="D688" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E688" s="36"/>
     </row>
     <row r="689" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A689" s="3" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B689" s="5"/>
       <c r="C689" s="5"/>
       <c r="D689" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E689" s="36"/>
     </row>
     <row r="690" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A690" s="3" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="B690" s="5"/>
       <c r="C690" s="5"/>
       <c r="D690" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E690" s="36"/>
     </row>
     <row r="691" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A691" s="3" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B691" s="5"/>
       <c r="C691" s="5"/>
       <c r="D691" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E691" s="36"/>
     </row>
     <row r="692" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A692" s="3" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B692" s="5"/>
       <c r="C692" s="5"/>
       <c r="D692" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E692" s="36"/>
     </row>
     <row r="693" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A693" s="3" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B693" s="5"/>
       <c r="C693" s="5"/>
       <c r="D693" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E693" s="36"/>
     </row>
     <row r="694" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A694" s="3" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B694" s="5"/>
       <c r="C694" s="5"/>
       <c r="D694" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E694" s="36"/>
     </row>
     <row r="695" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A695" s="3" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="B695" s="5"/>
       <c r="C695" s="5"/>
       <c r="D695" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E695" s="36"/>
     </row>
     <row r="696" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A696" s="3" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B696" s="5"/>
       <c r="C696" s="5"/>
       <c r="D696" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E696" s="36"/>
     </row>
     <row r="697" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A697" s="3" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="B697" s="5"/>
       <c r="C697" s="5"/>
       <c r="D697" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E697" s="36"/>
     </row>
     <row r="698" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A698" s="3" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B698" s="5"/>
       <c r="C698" s="5"/>
       <c r="D698" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E698" s="36"/>
     </row>
     <row r="699" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A699" s="3" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B699" s="5"/>
       <c r="C699" s="5"/>
       <c r="D699" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E699" s="36"/>
     </row>
     <row r="700" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A700" s="3" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B700" s="5"/>
       <c r="C700" s="5"/>
       <c r="D700" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E700" s="36"/>
     </row>
     <row r="701" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A701" s="3" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B701" s="5"/>
       <c r="C701" s="5"/>
       <c r="D701" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E701" s="36"/>
     </row>
     <row r="702" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A702" s="3" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B702" s="5"/>
       <c r="C702" s="5"/>
       <c r="D702" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E702" s="36"/>
     </row>
     <row r="703" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A703" s="3" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B703" s="5"/>
       <c r="C703" s="5"/>
       <c r="D703" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E703" s="36"/>
     </row>
     <row r="704" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A704" s="3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B704" s="5"/>
       <c r="C704" s="5"/>
       <c r="D704" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E704" s="36"/>
     </row>
     <row r="705" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A705" s="3" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B705" s="5"/>
       <c r="C705" s="5"/>
       <c r="D705" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E705" s="36"/>
     </row>
     <row r="706" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A706" s="3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B706" s="5"/>
       <c r="C706" s="5"/>
       <c r="D706" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E706" s="36"/>
     </row>
     <row r="707" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A707" s="3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B707" s="5"/>
       <c r="C707" s="5"/>
       <c r="D707" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E707" s="36"/>
     </row>
     <row r="708" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A708" s="3" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B708" s="5"/>
       <c r="C708" s="5"/>
       <c r="D708" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E708" s="36"/>
     </row>
     <row r="709" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A709" s="3" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B709" s="5"/>
       <c r="C709" s="5"/>
       <c r="D709" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E709" s="36"/>
     </row>
     <row r="710" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A710" s="3" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B710" s="5"/>
       <c r="C710" s="5"/>
       <c r="D710" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E710" s="36"/>
     </row>
     <row r="711" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A711" s="3" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B711" s="5"/>
       <c r="C711" s="5"/>
       <c r="D711" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E711" s="36"/>
     </row>
     <row r="712" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A712" s="3" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B712" s="5"/>
       <c r="C712" s="5"/>
       <c r="D712" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E712" s="36"/>
     </row>
     <row r="713" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A713" s="3" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B713" s="5"/>
       <c r="C713" s="5"/>
       <c r="D713" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E713" s="36"/>
     </row>
     <row r="714" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A714" s="3" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B714" s="5"/>
       <c r="C714" s="5"/>
       <c r="D714" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E714" s="36"/>
     </row>
     <row r="715" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A715" s="3" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B715" s="5"/>
       <c r="C715" s="5"/>
       <c r="D715" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E715" s="36"/>
     </row>
     <row r="716" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A716" s="3" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B716" s="5"/>
       <c r="C716" s="5"/>
       <c r="D716" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E716" s="36"/>
     </row>
     <row r="717" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A717" s="3" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B717" s="5"/>
       <c r="C717" s="5"/>
       <c r="D717" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E717" s="36"/>
     </row>
     <row r="718" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A718" s="3" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B718" s="5"/>
       <c r="C718" s="5"/>
       <c r="D718" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E718" s="36"/>
     </row>
     <row r="719" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A719" s="3" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B719" s="5"/>
       <c r="C719" s="5"/>
       <c r="D719" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E719" s="36"/>
     </row>
     <row r="720" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A720" s="3" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B720" s="5"/>
       <c r="C720" s="5"/>
       <c r="D720" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E720" s="36"/>
     </row>
     <row r="721" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A721" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B721" s="5"/>
       <c r="C721" s="5"/>
       <c r="D721" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E721" s="36"/>
     </row>
@@ -23737,7 +23767,7 @@
     </row>
     <row r="723" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A723" s="3" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B723" s="5"/>
       <c r="C723" s="5"/>
@@ -23746,7 +23776,7 @@
     </row>
     <row r="724" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A724" s="3" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B724" s="5"/>
       <c r="C724" s="5"/>
@@ -23755,7 +23785,7 @@
     </row>
     <row r="725" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A725" s="3" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B725" s="5"/>
       <c r="C725" s="5"/>
@@ -23764,7 +23794,7 @@
     </row>
     <row r="726" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A726" s="3" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="B726" s="5"/>
       <c r="C726" s="5"/>
@@ -23773,7 +23803,7 @@
     </row>
     <row r="727" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A727" s="3" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B727" s="5"/>
       <c r="C727" s="5"/>
@@ -23782,7 +23812,7 @@
     </row>
     <row r="728" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A728" s="3" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B728" s="5"/>
       <c r="C728" s="5"/>
@@ -23791,7 +23821,7 @@
     </row>
     <row r="729" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A729" s="3" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B729" s="5"/>
       <c r="C729" s="5"/>
@@ -23800,7 +23830,7 @@
     </row>
     <row r="730" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A730" s="3" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B730" s="5"/>
       <c r="C730" s="5"/>
@@ -23809,7 +23839,7 @@
     </row>
     <row r="731" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A731" s="3" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B731" s="5"/>
       <c r="C731" s="5"/>
@@ -23818,7 +23848,7 @@
     </row>
     <row r="732" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A732" s="3" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="B732" s="5"/>
       <c r="C732" s="5"/>
@@ -23827,7 +23857,7 @@
     </row>
     <row r="733" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A733" s="3" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B733" s="5"/>
       <c r="C733" s="5"/>
@@ -23836,7 +23866,7 @@
     </row>
     <row r="734" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A734" s="3" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="B734" s="5"/>
       <c r="C734" s="5"/>
@@ -23845,7 +23875,7 @@
     </row>
     <row r="735" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A735" s="3" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="B735" s="5"/>
       <c r="C735" s="5"/>
@@ -23861,7 +23891,7 @@
     </row>
     <row r="737" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A737" s="3" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="B737" s="5"/>
       <c r="C737" s="5"/>
@@ -23870,7 +23900,7 @@
     </row>
     <row r="738" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A738" s="3" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="B738" s="5"/>
       <c r="C738" s="5"/>
@@ -23879,7 +23909,7 @@
     </row>
     <row r="739" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A739" s="3" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B739" s="5"/>
       <c r="C739" s="5"/>
@@ -23888,7 +23918,7 @@
     </row>
     <row r="740" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A740" s="3" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B740" s="5"/>
       <c r="C740" s="5"/>
@@ -23897,7 +23927,7 @@
     </row>
     <row r="741" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A741" s="3" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B741" s="5"/>
       <c r="C741" s="5"/>
@@ -23906,7 +23936,7 @@
     </row>
     <row r="742" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A742" s="3" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B742" s="5"/>
       <c r="C742" s="5"/>
@@ -23915,7 +23945,7 @@
     </row>
     <row r="743" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A743" s="3" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="B743" s="5"/>
       <c r="C743" s="5"/>
@@ -23942,7 +23972,7 @@
     </row>
     <row r="746" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A746" s="3" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B746" s="5"/>
       <c r="C746" s="5"/>
@@ -23951,7 +23981,7 @@
     </row>
     <row r="747" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A747" s="3" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="B747" s="5"/>
       <c r="C747" s="5"/>
@@ -23960,7 +23990,7 @@
     </row>
     <row r="748" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A748" s="3" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="B748" s="5"/>
       <c r="C748" s="5"/>
@@ -23969,7 +23999,7 @@
     </row>
     <row r="749" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A749" s="3" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B749" s="5"/>
       <c r="C749" s="5"/>
@@ -23978,7 +24008,7 @@
     </row>
     <row r="750" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A750" s="3" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="B750" s="5"/>
       <c r="C750" s="5"/>
@@ -23987,7 +24017,7 @@
     </row>
     <row r="751" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A751" s="3" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="B751" s="5"/>
       <c r="C751" s="5"/>
@@ -23996,7 +24026,7 @@
     </row>
     <row r="752" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A752" s="3" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B752" s="5"/>
       <c r="C752" s="5"/>
@@ -24005,7 +24035,7 @@
     </row>
     <row r="753" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A753" s="3" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B753" s="5"/>
       <c r="C753" s="5"/>
@@ -24014,7 +24044,7 @@
     </row>
     <row r="754" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A754" s="3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B754" s="5"/>
       <c r="C754" s="5"/>
@@ -24023,7 +24053,7 @@
     </row>
     <row r="755" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A755" s="3" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="B755" s="5"/>
       <c r="C755" s="5"/>
@@ -24032,7 +24062,7 @@
     </row>
     <row r="756" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A756" s="3" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="B756" s="5"/>
       <c r="C756" s="5"/>
@@ -24041,7 +24071,7 @@
     </row>
     <row r="757" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A757" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="B757" s="5"/>
       <c r="C757" s="5"/>
@@ -24050,7 +24080,7 @@
     </row>
     <row r="758" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A758" s="3" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B758" s="5"/>
       <c r="C758" s="5"/>
@@ -24059,7 +24089,7 @@
     </row>
     <row r="759" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A759" s="3" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="B759" s="5"/>
       <c r="C759" s="5"/>
@@ -24068,7 +24098,7 @@
     </row>
     <row r="760" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A760" s="3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B760" s="5"/>
       <c r="C760" s="5"/>
@@ -24077,7 +24107,7 @@
     </row>
     <row r="761" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A761" s="3" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="B761" s="5"/>
       <c r="C761" s="5"/>
@@ -24086,7 +24116,7 @@
     </row>
     <row r="762" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A762" s="3" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="B762" s="5"/>
       <c r="C762" s="5"/>
@@ -24095,7 +24125,7 @@
     </row>
     <row r="763" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A763" s="3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B763" s="5"/>
       <c r="C763" s="5"/>
@@ -24104,7 +24134,7 @@
     </row>
     <row r="764" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A764" s="3" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="B764" s="5"/>
       <c r="C764" s="5"/>
@@ -24113,7 +24143,7 @@
     </row>
     <row r="765" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A765" s="3" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B765" s="5"/>
       <c r="C765" s="5"/>
@@ -24122,7 +24152,7 @@
     </row>
     <row r="766" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A766" s="3" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B766" s="5"/>
       <c r="C766" s="5"/>
@@ -24131,7 +24161,7 @@
     </row>
     <row r="767" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A767" s="3" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B767" s="5"/>
       <c r="C767" s="5"/>
@@ -24140,7 +24170,7 @@
     </row>
     <row r="768" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A768" s="3" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B768" s="5"/>
       <c r="C768" s="5"/>
@@ -24149,7 +24179,7 @@
     </row>
     <row r="769" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A769" s="3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B769" s="5"/>
       <c r="C769" s="5"/>
@@ -24158,7 +24188,7 @@
     </row>
     <row r="770" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A770" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="B770" s="5"/>
       <c r="C770" s="5"/>
@@ -24167,7 +24197,7 @@
     </row>
     <row r="771" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A771" s="3" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="B771" s="5"/>
       <c r="C771" s="5"/>
@@ -24176,7 +24206,7 @@
     </row>
     <row r="772" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A772" s="3" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="B772" s="5"/>
       <c r="C772" s="5"/>
@@ -24185,7 +24215,7 @@
     </row>
     <row r="773" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A773" s="3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="B773" s="5"/>
       <c r="C773" s="5"/>
@@ -24194,7 +24224,7 @@
     </row>
     <row r="774" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A774" s="3" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B774" s="5"/>
       <c r="C774" s="5"/>
@@ -24203,7 +24233,7 @@
     </row>
     <row r="775" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A775" s="3" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="B775" s="5"/>
       <c r="C775" s="5"/>
@@ -24212,7 +24242,7 @@
     </row>
     <row r="776" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A776" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="B776" s="5"/>
       <c r="C776" s="5"/>
@@ -24221,7 +24251,7 @@
     </row>
     <row r="777" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A777" s="3" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="B777" s="5"/>
       <c r="C777" s="5"/>
@@ -24230,7 +24260,7 @@
     </row>
     <row r="778" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A778" s="3" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B778" s="5"/>
       <c r="C778" s="5"/>
@@ -24239,7 +24269,7 @@
     </row>
     <row r="779" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A779" s="3" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="B779" s="5"/>
       <c r="C779" s="5"/>
@@ -24248,7 +24278,7 @@
     </row>
     <row r="780" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A780" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="B780" s="5"/>
       <c r="C780" s="5"/>
@@ -24257,7 +24287,7 @@
     </row>
     <row r="781" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A781" s="3" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B781" s="5"/>
       <c r="C781" s="5"/>
@@ -24266,7 +24296,7 @@
     </row>
     <row r="782" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A782" s="3" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="B782" s="5"/>
       <c r="C782" s="5"/>
@@ -24275,7 +24305,7 @@
     </row>
     <row r="783" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A783" s="3" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="B783" s="5"/>
       <c r="C783" s="5"/>
@@ -24284,7 +24314,7 @@
     </row>
     <row r="784" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A784" s="3" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="B784" s="5"/>
       <c r="C784" s="5"/>
@@ -24293,7 +24323,7 @@
     </row>
     <row r="785" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A785" s="3" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="B785" s="5"/>
       <c r="C785" s="5"/>
@@ -24302,7 +24332,7 @@
     </row>
     <row r="786" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A786" s="3" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="B786" s="5"/>
       <c r="C786" s="5"/>
@@ -24311,7 +24341,7 @@
     </row>
     <row r="787" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A787" s="3" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="B787" s="5"/>
       <c r="C787" s="5"/>
@@ -24320,7 +24350,7 @@
     </row>
     <row r="788" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A788" s="3" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B788" s="5"/>
       <c r="C788" s="5"/>
@@ -24329,7 +24359,7 @@
     </row>
     <row r="789" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A789" s="3" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="B789" s="5"/>
       <c r="C789" s="5"/>
@@ -24345,7 +24375,7 @@
     </row>
     <row r="791" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A791" s="3" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="B791" s="5"/>
       <c r="C791" s="5"/>
@@ -24354,7 +24384,7 @@
     </row>
     <row r="792" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A792" s="3" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="B792" s="5"/>
       <c r="C792" s="5"/>
@@ -24363,7 +24393,7 @@
     </row>
     <row r="793" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A793" s="3" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="B793" s="5"/>
       <c r="C793" s="5"/>
@@ -24372,7 +24402,7 @@
     </row>
     <row r="794" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A794" s="3" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="B794" s="5"/>
       <c r="C794" s="5"/>
@@ -24381,7 +24411,7 @@
     </row>
     <row r="795" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A795" s="3" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="B795" s="5"/>
       <c r="C795" s="5"/>
@@ -24390,7 +24420,7 @@
     </row>
     <row r="796" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A796" s="3" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="B796" s="5"/>
       <c r="C796" s="5"/>
@@ -24399,7 +24429,7 @@
     </row>
     <row r="797" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A797" s="3" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="B797" s="5"/>
       <c r="C797" s="5"/>
@@ -24408,7 +24438,7 @@
     </row>
     <row r="798" spans="1:5" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A798" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="B798" s="5"/>
       <c r="C798" s="5"/>

</xml_diff>

<commit_message>
Updates for test cases and creates newest jar versions, without clipboard feature
</commit_message>
<xml_diff>
--- a/libs/ReferenceData/Maple.xlsx
+++ b/libs/ReferenceData/Maple.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2672" uniqueCount="1181">
   <si>
     <t>Maple</t>
   </si>
@@ -3552,6 +3552,21 @@
   </si>
   <si>
     <t>X3:LegendreQXexp(-($0)*Pi*I)*LegendreQ($1,$0,$2)/GAMMA($1+$0+1)</t>
+  </si>
+  <si>
+    <t>complex</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>rational</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>posint</t>
   </si>
 </sst>
 </file>
@@ -16222,8 +16237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W799"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
-      <selection activeCell="B404" sqref="B404"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17558,8 +17573,12 @@
       <c r="A115" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
+      <c r="B115" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C115" s="5">
+        <v>0</v>
+      </c>
       <c r="D115" s="5"/>
       <c r="E115" s="36"/>
     </row>
@@ -17567,8 +17586,12 @@
       <c r="A116" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
+      <c r="B116" s="5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C116" s="5">
+        <v>0</v>
+      </c>
       <c r="D116" s="5"/>
       <c r="E116" s="36"/>
     </row>
@@ -17576,8 +17599,12 @@
       <c r="A117" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
+      <c r="B117" s="5" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C117" s="5">
+        <v>0</v>
+      </c>
       <c r="D117" s="5"/>
       <c r="E117" s="36"/>
     </row>
@@ -17585,8 +17612,12 @@
       <c r="A118" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
+      <c r="B118" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C118" s="5">
+        <v>0</v>
+      </c>
       <c r="D118" s="5"/>
       <c r="E118" s="36"/>
     </row>
@@ -17594,8 +17625,12 @@
       <c r="A119" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
+      <c r="B119" s="5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C119" s="5">
+        <v>0</v>
+      </c>
       <c r="D119" s="5"/>
       <c r="E119" s="36"/>
     </row>

</xml_diff>

<commit_message>
Ad-hoc changes for the thesis and numerical tests.
</commit_message>
<xml_diff>
--- a/libs/ReferenceData/Maple.xlsx
+++ b/libs/ReferenceData/Maple.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -3644,7 +3644,7 @@
     <t>X1:\pderivX\pderiv[$0]{$1}{$2}</t>
   </si>
   <si>
-    <t>diff($1, [$2$$0])</t>
+    <t>diff($1, [$2$($0)])</t>
   </si>
 </sst>
 </file>
@@ -16342,8 +16342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="F278" sqref="F278:F282"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bug fix in created jars
</commit_message>
<xml_diff>
--- a/libs/ReferenceData/Maple.xlsx
+++ b/libs/ReferenceData/Maple.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10550" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10550" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maple2LaTeX" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="1205">
   <si>
     <t>Maple</t>
   </si>
@@ -3327,12 +3327,6 @@
   </si>
   <si>
     <t>int((1-cos(t))/t, t = 0 .. $0)</t>
-  </si>
-  <si>
-    <t>int(sech(t), t = 0 .. $0)</t>
-  </si>
-  <si>
-    <t>int(sec(t), t = 0 .. $0)</t>
   </si>
   <si>
     <t>Ei($0)+ln($0)+gamma</t>
@@ -3650,7 +3644,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -4304,10 +4298,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z804"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A620" sqref="A620"/>
     </sheetView>
   </sheetViews>
@@ -4335,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -5085,7 +5079,7 @@
     <row r="46" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
@@ -5097,7 +5091,7 @@
     <row r="47" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
@@ -5994,10 +5988,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C100" s="5">
         <v>2</v>
@@ -6007,15 +6001,15 @@
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
       <c r="H100" s="48" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C101" s="5">
         <v>2</v>
@@ -6025,12 +6019,12 @@
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
       <c r="H101" s="48" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -6039,7 +6033,7 @@
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
       <c r="H102" s="48" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
@@ -9203,7 +9197,7 @@
         <v>517</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C323" s="5">
         <v>1</v>
@@ -9291,7 +9285,7 @@
         <v>529</v>
       </c>
       <c r="B329" s="29" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C329" s="5">
         <v>6</v>
@@ -10425,7 +10419,7 @@
     <row r="399" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A399" s="3"/>
       <c r="B399" s="36" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="C399" s="5"/>
       <c r="D399" s="5"/>
@@ -10437,7 +10431,7 @@
     <row r="400" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A400" s="3"/>
       <c r="B400" s="36" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C400" s="5"/>
       <c r="D400" s="5"/>
@@ -10449,7 +10443,7 @@
     <row r="401" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A401" s="5"/>
       <c r="B401" s="36" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C401" s="5"/>
       <c r="D401" s="5"/>
@@ -10461,7 +10455,7 @@
     <row r="402" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A402" s="5"/>
       <c r="B402" s="36" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C402" s="5"/>
       <c r="D402" s="5"/>
@@ -10472,21 +10466,21 @@
     </row>
     <row r="403" spans="1:8" ht="121.5" x14ac:dyDescent="0.3">
       <c r="A403" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B403" s="3" t="s">
         <v>1112</v>
-      </c>
-      <c r="B403" s="3" t="s">
-        <v>1114</v>
       </c>
       <c r="C403" s="5">
         <v>2</v>
       </c>
       <c r="D403" s="3" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="E403" s="5"/>
       <c r="F403" s="5"/>
       <c r="G403" s="5" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="H403" s="6" t="s">
         <v>656</v>
@@ -10494,21 +10488,21 @@
     </row>
     <row r="404" spans="1:8" ht="81" x14ac:dyDescent="0.3">
       <c r="A404" s="3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C404" s="5">
         <v>3</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="E404" s="5"/>
       <c r="F404" s="5"/>
       <c r="G404" s="5" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="H404" s="6" t="s">
         <v>656</v>
@@ -10516,21 +10510,21 @@
     </row>
     <row r="405" spans="1:8" ht="81" x14ac:dyDescent="0.3">
       <c r="A405" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B405" s="3" t="s">
         <v>1113</v>
-      </c>
-      <c r="B405" s="3" t="s">
-        <v>1115</v>
       </c>
       <c r="C405" s="5">
         <v>2</v>
       </c>
       <c r="D405" s="3" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E405" s="5"/>
       <c r="F405" s="5"/>
       <c r="G405" s="5" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="H405" s="6" t="s">
         <v>657</v>
@@ -10538,21 +10532,21 @@
     </row>
     <row r="406" spans="1:8" ht="81" x14ac:dyDescent="0.3">
       <c r="A406" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C406" s="5">
         <v>3</v>
       </c>
       <c r="D406" s="3" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E406" s="5"/>
       <c r="F406" s="5"/>
       <c r="G406" s="5" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="H406" s="6" t="s">
         <v>657</v>
@@ -10561,7 +10555,7 @@
     <row r="407" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A407" s="5"/>
       <c r="B407" s="36" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C407" s="5"/>
       <c r="D407" s="5"/>
@@ -10573,7 +10567,7 @@
     <row r="408" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A408" s="5"/>
       <c r="B408" s="36" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C408" s="5"/>
       <c r="D408" s="5"/>
@@ -10585,7 +10579,7 @@
     <row r="409" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A409" s="5"/>
       <c r="B409" s="42" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C409" s="5"/>
       <c r="D409" s="5"/>
@@ -10599,7 +10593,7 @@
     <row r="410" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A410" s="5"/>
       <c r="B410" s="42" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="C410" s="5"/>
       <c r="D410" s="5"/>
@@ -13556,10 +13550,10 @@
     </row>
     <row r="619" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A619" s="3" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="B619" s="3" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="C619" s="5">
         <v>2</v>
@@ -13568,7 +13562,7 @@
       <c r="E619" s="5"/>
       <c r="F619" s="5"/>
       <c r="G619" s="3" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="H619" s="6" t="s">
         <v>933</v>
@@ -13579,7 +13573,7 @@
         <v>931</v>
       </c>
       <c r="B620" s="3" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C620" s="5">
         <v>3</v>
@@ -16098,240 +16092,240 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
-    <hyperlink ref="H9" r:id="rId7"/>
-    <hyperlink ref="H10" r:id="rId8"/>
-    <hyperlink ref="H11" r:id="rId9"/>
-    <hyperlink ref="H12" r:id="rId10"/>
-    <hyperlink ref="H13" r:id="rId11"/>
-    <hyperlink ref="H14" r:id="rId12"/>
-    <hyperlink ref="H16" r:id="rId13"/>
-    <hyperlink ref="H17" r:id="rId14"/>
-    <hyperlink ref="H18" r:id="rId15"/>
-    <hyperlink ref="H19" r:id="rId16"/>
-    <hyperlink ref="H20" r:id="rId17"/>
-    <hyperlink ref="H21" r:id="rId18"/>
-    <hyperlink ref="H22" r:id="rId19"/>
-    <hyperlink ref="H24" r:id="rId20"/>
-    <hyperlink ref="H25" r:id="rId21"/>
-    <hyperlink ref="H26" r:id="rId22"/>
-    <hyperlink ref="H27" r:id="rId23"/>
-    <hyperlink ref="H28" r:id="rId24"/>
-    <hyperlink ref="H29" r:id="rId25"/>
-    <hyperlink ref="H31" r:id="rId26"/>
-    <hyperlink ref="H32" r:id="rId27"/>
-    <hyperlink ref="H33" r:id="rId28"/>
-    <hyperlink ref="H35" r:id="rId29"/>
-    <hyperlink ref="H37" r:id="rId30"/>
-    <hyperlink ref="H38" r:id="rId31"/>
-    <hyperlink ref="H40" r:id="rId32"/>
-    <hyperlink ref="H41" r:id="rId33"/>
-    <hyperlink ref="H42" r:id="rId34"/>
-    <hyperlink ref="H43" r:id="rId35"/>
-    <hyperlink ref="H44" r:id="rId36"/>
-    <hyperlink ref="H49" r:id="rId37"/>
-    <hyperlink ref="H50" r:id="rId38"/>
-    <hyperlink ref="H51" r:id="rId39"/>
-    <hyperlink ref="H52" r:id="rId40"/>
-    <hyperlink ref="H53" r:id="rId41"/>
-    <hyperlink ref="H55" r:id="rId42"/>
-    <hyperlink ref="H57" r:id="rId43"/>
-    <hyperlink ref="H58" r:id="rId44"/>
-    <hyperlink ref="H59" r:id="rId45"/>
-    <hyperlink ref="H60" r:id="rId46"/>
-    <hyperlink ref="H61" r:id="rId47"/>
-    <hyperlink ref="H62" r:id="rId48"/>
-    <hyperlink ref="H64" r:id="rId49"/>
-    <hyperlink ref="H65" r:id="rId50"/>
-    <hyperlink ref="H66" r:id="rId51"/>
-    <hyperlink ref="H67" r:id="rId52"/>
-    <hyperlink ref="H68" r:id="rId53"/>
-    <hyperlink ref="H69" r:id="rId54"/>
-    <hyperlink ref="H70" r:id="rId55"/>
-    <hyperlink ref="H71" r:id="rId56"/>
-    <hyperlink ref="H72" r:id="rId57"/>
-    <hyperlink ref="H73" r:id="rId58"/>
-    <hyperlink ref="H74" r:id="rId59"/>
-    <hyperlink ref="H75" r:id="rId60"/>
-    <hyperlink ref="H76" r:id="rId61"/>
-    <hyperlink ref="H78" r:id="rId62"/>
-    <hyperlink ref="H79" r:id="rId63"/>
-    <hyperlink ref="H82" r:id="rId64"/>
-    <hyperlink ref="H83" r:id="rId65"/>
-    <hyperlink ref="H84" r:id="rId66"/>
-    <hyperlink ref="H85" r:id="rId67"/>
-    <hyperlink ref="H86" r:id="rId68"/>
-    <hyperlink ref="H87" r:id="rId69"/>
-    <hyperlink ref="H88" r:id="rId70"/>
-    <hyperlink ref="H89" r:id="rId71"/>
-    <hyperlink ref="H90" r:id="rId72"/>
-    <hyperlink ref="H91" r:id="rId73"/>
-    <hyperlink ref="H92" r:id="rId74"/>
-    <hyperlink ref="H93" r:id="rId75"/>
-    <hyperlink ref="H96" r:id="rId76"/>
-    <hyperlink ref="H105" r:id="rId77"/>
-    <hyperlink ref="H111" r:id="rId78"/>
-    <hyperlink ref="H112" r:id="rId79"/>
-    <hyperlink ref="H115" r:id="rId80"/>
-    <hyperlink ref="H116" r:id="rId81"/>
-    <hyperlink ref="H125" r:id="rId82"/>
-    <hyperlink ref="H126" r:id="rId83"/>
-    <hyperlink ref="H127" r:id="rId84"/>
-    <hyperlink ref="H128" r:id="rId85"/>
-    <hyperlink ref="H129" r:id="rId86"/>
-    <hyperlink ref="H132" r:id="rId87"/>
-    <hyperlink ref="H134" r:id="rId88"/>
-    <hyperlink ref="H144" r:id="rId89"/>
-    <hyperlink ref="H145" r:id="rId90"/>
-    <hyperlink ref="H161" r:id="rId91"/>
-    <hyperlink ref="H162" r:id="rId92"/>
-    <hyperlink ref="H170" r:id="rId93"/>
-    <hyperlink ref="H171" r:id="rId94"/>
-    <hyperlink ref="H172" r:id="rId95"/>
-    <hyperlink ref="H173" r:id="rId96"/>
-    <hyperlink ref="H184" r:id="rId97"/>
-    <hyperlink ref="H185" r:id="rId98"/>
-    <hyperlink ref="H206" r:id="rId99"/>
-    <hyperlink ref="H228" r:id="rId100"/>
-    <hyperlink ref="H243" r:id="rId101"/>
-    <hyperlink ref="H245" r:id="rId102"/>
-    <hyperlink ref="H247" r:id="rId103"/>
-    <hyperlink ref="H249" r:id="rId104"/>
-    <hyperlink ref="H253" r:id="rId105"/>
-    <hyperlink ref="H261" r:id="rId106"/>
-    <hyperlink ref="H264" r:id="rId107"/>
-    <hyperlink ref="H266" r:id="rId108"/>
-    <hyperlink ref="H286" r:id="rId109"/>
-    <hyperlink ref="H289" r:id="rId110"/>
-    <hyperlink ref="H290" r:id="rId111"/>
-    <hyperlink ref="H291" r:id="rId112"/>
-    <hyperlink ref="H295" r:id="rId113"/>
-    <hyperlink ref="H301" r:id="rId114"/>
-    <hyperlink ref="H302" r:id="rId115"/>
-    <hyperlink ref="H303" r:id="rId116"/>
-    <hyperlink ref="H304" r:id="rId117"/>
-    <hyperlink ref="H306" r:id="rId118"/>
-    <hyperlink ref="H307" r:id="rId119"/>
-    <hyperlink ref="H308" r:id="rId120"/>
-    <hyperlink ref="H309" r:id="rId121"/>
-    <hyperlink ref="H310" r:id="rId122"/>
-    <hyperlink ref="H311" r:id="rId123"/>
-    <hyperlink ref="H318" r:id="rId124"/>
-    <hyperlink ref="H323" r:id="rId125"/>
-    <hyperlink ref="H324" r:id="rId126"/>
-    <hyperlink ref="H327" r:id="rId127"/>
-    <hyperlink ref="H329" r:id="rId128"/>
-    <hyperlink ref="H330" r:id="rId129"/>
-    <hyperlink ref="H331" r:id="rId130"/>
-    <hyperlink ref="H332" r:id="rId131"/>
-    <hyperlink ref="H333" r:id="rId132"/>
-    <hyperlink ref="H336" r:id="rId133"/>
-    <hyperlink ref="H337" r:id="rId134"/>
-    <hyperlink ref="H338" r:id="rId135"/>
-    <hyperlink ref="H342" r:id="rId136"/>
-    <hyperlink ref="H343" r:id="rId137"/>
-    <hyperlink ref="H353" r:id="rId138"/>
-    <hyperlink ref="H354" r:id="rId139"/>
-    <hyperlink ref="H355" r:id="rId140"/>
-    <hyperlink ref="H356" r:id="rId141"/>
-    <hyperlink ref="H357" r:id="rId142"/>
-    <hyperlink ref="H358" r:id="rId143"/>
-    <hyperlink ref="H359" r:id="rId144"/>
-    <hyperlink ref="H360" r:id="rId145"/>
-    <hyperlink ref="H361" r:id="rId146"/>
-    <hyperlink ref="H362" r:id="rId147"/>
-    <hyperlink ref="H363" r:id="rId148"/>
-    <hyperlink ref="H364" r:id="rId149"/>
-    <hyperlink ref="H365" r:id="rId150"/>
-    <hyperlink ref="H366" r:id="rId151"/>
-    <hyperlink ref="H367" r:id="rId152"/>
-    <hyperlink ref="H368" r:id="rId153"/>
-    <hyperlink ref="H369" r:id="rId154"/>
-    <hyperlink ref="H370" r:id="rId155"/>
-    <hyperlink ref="H371" r:id="rId156"/>
-    <hyperlink ref="H372" r:id="rId157"/>
-    <hyperlink ref="H373" r:id="rId158"/>
-    <hyperlink ref="H374" r:id="rId159"/>
-    <hyperlink ref="H375" r:id="rId160"/>
-    <hyperlink ref="H376" r:id="rId161"/>
-    <hyperlink ref="H377" r:id="rId162"/>
-    <hyperlink ref="H379" r:id="rId163"/>
-    <hyperlink ref="H380" r:id="rId164"/>
-    <hyperlink ref="H381" r:id="rId165"/>
-    <hyperlink ref="H382" r:id="rId166"/>
-    <hyperlink ref="H383" r:id="rId167"/>
-    <hyperlink ref="H386" r:id="rId168"/>
-    <hyperlink ref="H389" r:id="rId169"/>
-    <hyperlink ref="H390" r:id="rId170"/>
-    <hyperlink ref="H391" r:id="rId171"/>
-    <hyperlink ref="H392" r:id="rId172"/>
-    <hyperlink ref="H412" r:id="rId173"/>
-    <hyperlink ref="H413" r:id="rId174"/>
-    <hyperlink ref="H414" r:id="rId175"/>
-    <hyperlink ref="H416" r:id="rId176"/>
-    <hyperlink ref="H417" r:id="rId177"/>
-    <hyperlink ref="H418" r:id="rId178"/>
-    <hyperlink ref="H420" r:id="rId179"/>
-    <hyperlink ref="H421" r:id="rId180"/>
-    <hyperlink ref="H423" r:id="rId181"/>
-    <hyperlink ref="H425" r:id="rId182"/>
-    <hyperlink ref="H426" r:id="rId183"/>
-    <hyperlink ref="H428" r:id="rId184"/>
-    <hyperlink ref="H429" r:id="rId185"/>
-    <hyperlink ref="H431" r:id="rId186"/>
-    <hyperlink ref="H432" r:id="rId187"/>
-    <hyperlink ref="H457" r:id="rId188"/>
-    <hyperlink ref="H459" r:id="rId189"/>
-    <hyperlink ref="H472" r:id="rId190"/>
-    <hyperlink ref="H476" r:id="rId191"/>
-    <hyperlink ref="H488" r:id="rId192"/>
-    <hyperlink ref="H489" r:id="rId193"/>
-    <hyperlink ref="H491" r:id="rId194"/>
-    <hyperlink ref="H493" r:id="rId195"/>
-    <hyperlink ref="H496" r:id="rId196"/>
-    <hyperlink ref="H497" r:id="rId197"/>
-    <hyperlink ref="H499" r:id="rId198"/>
-    <hyperlink ref="H501" r:id="rId199"/>
-    <hyperlink ref="H510" r:id="rId200"/>
-    <hyperlink ref="H511" r:id="rId201"/>
-    <hyperlink ref="H512" r:id="rId202"/>
-    <hyperlink ref="H513" r:id="rId203"/>
-    <hyperlink ref="H518" r:id="rId204"/>
-    <hyperlink ref="H519" r:id="rId205"/>
-    <hyperlink ref="H520" r:id="rId206"/>
-    <hyperlink ref="H530" r:id="rId207"/>
-    <hyperlink ref="H532" r:id="rId208"/>
-    <hyperlink ref="H534" r:id="rId209"/>
-    <hyperlink ref="H537" r:id="rId210"/>
-    <hyperlink ref="H538" r:id="rId211"/>
-    <hyperlink ref="H540" r:id="rId212"/>
-    <hyperlink ref="H541" r:id="rId213"/>
-    <hyperlink ref="H542" r:id="rId214"/>
-    <hyperlink ref="H544" r:id="rId215"/>
-    <hyperlink ref="H557" r:id="rId216"/>
-    <hyperlink ref="H562" r:id="rId217"/>
-    <hyperlink ref="H572" r:id="rId218"/>
-    <hyperlink ref="H573" r:id="rId219"/>
-    <hyperlink ref="H587" r:id="rId220"/>
-    <hyperlink ref="H591" r:id="rId221"/>
-    <hyperlink ref="H592" r:id="rId222"/>
-    <hyperlink ref="H602" r:id="rId223"/>
-    <hyperlink ref="H603" r:id="rId224"/>
-    <hyperlink ref="H609" r:id="rId225"/>
-    <hyperlink ref="H610" r:id="rId226"/>
-    <hyperlink ref="H619" r:id="rId227"/>
-    <hyperlink ref="H406" r:id="rId228"/>
-    <hyperlink ref="H404" r:id="rId229"/>
-    <hyperlink ref="H403" r:id="rId230"/>
-    <hyperlink ref="H405" r:id="rId231"/>
-    <hyperlink ref="H102" r:id="rId232"/>
-    <hyperlink ref="H100" r:id="rId233"/>
-    <hyperlink ref="H101" r:id="rId234"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="H29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H35" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H37" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H38" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H40" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H41" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H42" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H43" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H44" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H49" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="H51" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H52" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H53" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H55" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H57" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="H58" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H59" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="H60" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="H61" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="H62" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="H64" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="H65" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="H66" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="H67" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="H68" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="H69" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="H70" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="H71" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="H72" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="H73" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="H74" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H75" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="H76" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="H78" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="H79" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="H82" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="H83" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="H84" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="H85" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="H86" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="H87" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="H88" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="H89" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="H90" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="H91" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="H92" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="H93" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="H96" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="H105" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="H111" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="H112" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="H115" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="H116" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="H125" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="H126" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="H127" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="H128" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="H129" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="H132" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="H134" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="H144" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="H145" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="H161" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="H162" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="H170" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="H171" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="H172" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="H173" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="H184" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="H185" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="H206" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="H228" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="H243" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="H245" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="H247" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="H249" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="H253" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="H261" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="H264" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="H266" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="H286" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="H289" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="H290" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="H291" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="H295" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="H301" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="H302" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="H303" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="H304" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="H306" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="H307" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="H308" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="H309" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="H310" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="H311" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="H318" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="H323" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="H324" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="H327" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="H329" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="H330" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="H331" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="H332" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="H333" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="H336" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="H337" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="H338" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="H342" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="H343" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="H353" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="H354" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="H355" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="H356" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="H357" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="H358" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="H359" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="H360" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="H361" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="H362" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="H363" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="H364" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="H365" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="H366" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="H367" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="H368" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="H369" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="H370" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="H371" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="H372" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="H373" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="H374" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="H375" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="H376" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="H377" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="H379" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="H380" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="H381" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="H382" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="H383" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="H386" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="H389" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="H390" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="H391" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="H392" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="H412" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="H413" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="H414" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="H416" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="H417" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="H418" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="H420" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="H421" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="H423" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="H425" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="H426" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="H428" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="H429" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="H431" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="H432" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="H457" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="H459" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="H472" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="H476" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="H488" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="H489" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="H491" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="H493" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="H496" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="H497" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="H499" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="H501" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="H510" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="H511" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="H512" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="H513" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="H518" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="H519" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="H520" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="H530" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="H532" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="H534" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="H537" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="H538" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="H540" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="H541" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="H542" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="H544" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="H557" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="H562" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="H572" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="H573" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="H587" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="H591" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="H592" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="H602" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="H603" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="H609" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="H610" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="H619" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="H406" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="H404" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="H403" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="H405" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="H102" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="H100" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="H101" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="25" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId235"/>
@@ -16339,11 +16333,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16368,10 +16362,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>1098</v>
@@ -16849,32 +16843,32 @@
     </row>
     <row r="38" spans="1:6" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>1200</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>1202</v>
       </c>
       <c r="C38" s="4">
         <v>2</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="36"/>
     </row>
     <row r="39" spans="1:6" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>1201</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>1203</v>
       </c>
       <c r="C39" s="4">
         <v>2</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="36"/>
@@ -16969,26 +16963,26 @@
     </row>
     <row r="47" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="3" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="3" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="13.5" x14ac:dyDescent="0.3">
@@ -17013,7 +17007,9 @@
         <v>113</v>
       </c>
       <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="F50" s="37" t="s">
+        <v>1101</v>
+      </c>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
@@ -17061,9 +17057,7 @@
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
-      <c r="F52" s="37" t="s">
-        <v>1102</v>
-      </c>
+      <c r="F52" s="37"/>
     </row>
     <row r="53" spans="1:24" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
@@ -17115,9 +17109,7 @@
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
-      <c r="F56" s="37" t="s">
-        <v>1103</v>
-      </c>
+      <c r="F56" s="37"/>
     </row>
     <row r="57" spans="1:24" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
@@ -17163,7 +17155,7 @@
         <v>140</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="F60" s="36"/>
     </row>
@@ -17179,7 +17171,7 @@
         <v>140</v>
       </c>
       <c r="E61" s="17" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="F61" s="36"/>
     </row>
@@ -17195,7 +17187,7 @@
         <v>140</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="F62" s="36"/>
     </row>
@@ -17211,7 +17203,7 @@
         <v>140</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="F63" s="36"/>
     </row>
@@ -17252,7 +17244,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="3"/>
@@ -17326,16 +17318,16 @@
         <v>1</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>171</v>
@@ -17375,7 +17367,7 @@
         <v>180</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="F73" s="36"/>
     </row>
@@ -17486,7 +17478,7 @@
         <v>205</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C84" s="5">
         <v>4</v>
@@ -17540,7 +17532,7 @@
         <v>214</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="C90" s="5">
         <v>4</v>
@@ -17575,14 +17567,14 @@
     </row>
     <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
@@ -17691,7 +17683,7 @@
         <v>230</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="F104" s="36"/>
     </row>
@@ -17775,10 +17767,10 @@
     </row>
     <row r="112" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>1204</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>1206</v>
       </c>
       <c r="C112" s="5">
         <v>2</v>
@@ -17789,10 +17781,10 @@
     </row>
     <row r="113" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C113" s="5">
         <v>2</v>
@@ -17864,7 +17856,7 @@
         <v>249</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="C119" s="5">
         <v>0</v>
@@ -17878,7 +17870,7 @@
         <v>250</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="C120" s="5">
         <v>0</v>
@@ -17892,7 +17884,7 @@
         <v>251</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="C121" s="5">
         <v>0</v>
@@ -17906,7 +17898,7 @@
         <v>252</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="C122" s="5">
         <v>0</v>
@@ -17920,7 +17912,7 @@
         <v>253</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="C123" s="5">
         <v>0</v>
@@ -17951,7 +17943,7 @@
     </row>
     <row r="126" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>256</v>
@@ -17985,7 +17977,7 @@
     </row>
     <row r="129" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>263</v>
@@ -17999,7 +17991,7 @@
     </row>
     <row r="130" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>266</v>
@@ -18041,7 +18033,7 @@
         <v>272</v>
       </c>
       <c r="E133" s="17" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="F133" s="36"/>
     </row>
@@ -18069,7 +18061,7 @@
         <v>277</v>
       </c>
       <c r="E135" s="17" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="F135" s="36"/>
     </row>
@@ -19449,7 +19441,7 @@
         <v>431</v>
       </c>
       <c r="E265" s="17" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F265" s="16" t="s">
         <v>429</v>
@@ -19477,7 +19469,7 @@
         <v>431</v>
       </c>
       <c r="E267" s="17" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F267" s="16" t="s">
         <v>434</v>
@@ -19683,7 +19675,7 @@
         <v>455</v>
       </c>
       <c r="E287" s="17" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F287" s="39" t="s">
         <v>456</v>
@@ -20354,7 +20346,7 @@
         <v>558</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C343" s="5">
         <v>3</v>
@@ -20368,7 +20360,7 @@
         <v>561</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C344" s="5">
         <v>3</v>
@@ -20849,10 +20841,10 @@
     </row>
     <row r="380" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A380" s="3" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="B380" s="32" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C380" s="5">
         <v>2</v>
@@ -20896,7 +20888,7 @@
       </c>
       <c r="E384" s="43"/>
       <c r="F384" s="53" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="385" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
@@ -20918,7 +20910,7 @@
       <c r="D386" s="5"/>
       <c r="E386" s="5"/>
       <c r="F386" s="37" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="387" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
@@ -21067,138 +21059,138 @@
     </row>
     <row r="400" spans="1:6" ht="108" x14ac:dyDescent="0.3">
       <c r="A400" s="36" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C400" s="5">
         <v>2</v>
       </c>
       <c r="D400" s="36" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E400" s="36"/>
       <c r="F400" s="36"/>
     </row>
     <row r="401" spans="1:6" ht="108" x14ac:dyDescent="0.3">
       <c r="A401" s="36" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C401" s="5">
         <v>3</v>
       </c>
       <c r="D401" s="36" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E401" s="36"/>
       <c r="F401" s="36"/>
     </row>
     <row r="402" spans="1:6" ht="108" x14ac:dyDescent="0.3">
       <c r="A402" s="36" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C402" s="5">
         <v>2</v>
       </c>
       <c r="D402" s="36" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E402" s="36"/>
       <c r="F402" s="36"/>
     </row>
     <row r="403" spans="1:6" ht="108" x14ac:dyDescent="0.3">
       <c r="A403" s="36" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C403" s="5">
         <v>3</v>
       </c>
       <c r="D403" s="36" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E403" s="36"/>
       <c r="F403" s="36"/>
     </row>
     <row r="404" spans="1:6" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A404" s="3" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C404" s="5">
         <v>2</v>
       </c>
       <c r="D404" s="36" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="E404" s="36"/>
       <c r="F404" s="36"/>
     </row>
     <row r="405" spans="1:6" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A405" s="3" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C405" s="5">
         <v>3</v>
       </c>
       <c r="D405" s="36" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="E405" s="36"/>
       <c r="F405" s="3"/>
     </row>
     <row r="406" spans="1:6" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A406" s="3" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C406" s="5">
         <v>2</v>
       </c>
       <c r="D406" s="36" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="E406" s="36"/>
       <c r="F406" s="36"/>
     </row>
     <row r="407" spans="1:6" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A407" s="3" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C407" s="5">
         <v>3</v>
       </c>
       <c r="D407" s="36" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="E407" s="36"/>
       <c r="F407" s="36"/>
     </row>
     <row r="408" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A408" s="36" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="B408" s="5" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="C408" s="5">
         <v>2</v>
@@ -21209,10 +21201,10 @@
     </row>
     <row r="409" spans="1:6" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A409" s="36" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="B409" s="5" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="C409" s="5">
         <v>3</v>
@@ -21223,7 +21215,7 @@
     </row>
     <row r="410" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A410" s="42" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="B410" s="5"/>
       <c r="C410" s="5"/>
@@ -21233,7 +21225,7 @@
     </row>
     <row r="411" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A411" s="42" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="B411" s="5"/>
       <c r="C411" s="5"/>
@@ -21251,7 +21243,7 @@
     </row>
     <row r="413" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A413" s="16" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="B413" s="16" t="s">
         <v>658</v>
@@ -21267,7 +21259,7 @@
     </row>
     <row r="414" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A414" s="16" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="B414" s="16" t="s">
         <v>662</v>
@@ -21283,7 +21275,7 @@
     </row>
     <row r="415" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A415" s="16" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="B415" s="16" t="s">
         <v>665</v>
@@ -21306,7 +21298,7 @@
       <c r="D416" s="3"/>
       <c r="E416" s="3"/>
       <c r="F416" s="37" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="417" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
@@ -21353,7 +21345,7 @@
     </row>
     <row r="420" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A420" s="36" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="B420" s="5"/>
       <c r="C420" s="5">
@@ -21362,7 +21354,7 @@
       <c r="D420" s="3"/>
       <c r="E420" s="3"/>
       <c r="F420" s="37" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="421" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
@@ -21958,7 +21950,7 @@
       </c>
       <c r="E476" s="3"/>
       <c r="F476" s="54" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="477" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
@@ -22146,7 +22138,7 @@
         <v>773</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="C493" s="5">
         <v>2</v>
@@ -22174,7 +22166,7 @@
         <v>777</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C495" s="5">
         <v>2</v>
@@ -22880,7 +22872,7 @@
         <v>864</v>
       </c>
       <c r="B558" s="3" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C558" s="5">
         <v>2</v>
@@ -23454,7 +23446,7 @@
       <c r="D612" s="5"/>
       <c r="E612" s="5"/>
       <c r="F612" s="37" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="613" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
@@ -23525,10 +23517,10 @@
     </row>
     <row r="620" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A620" s="3" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="B620" s="3" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="C620" s="5">
         <v>2</v>
@@ -23539,7 +23531,7 @@
     </row>
     <row r="621" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A621" s="3" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="B621" s="3" t="s">
         <v>931</v>
@@ -23553,10 +23545,10 @@
     </row>
     <row r="622" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A622" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B622" s="3" t="s">
         <v>1176</v>
-      </c>
-      <c r="B622" s="3" t="s">
-        <v>1178</v>
       </c>
       <c r="C622" s="5">
         <v>2</v>
@@ -23567,7 +23559,7 @@
     </row>
     <row r="623" spans="1:6" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A623" s="3" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="B623" s="3" t="s">
         <v>931</v>
@@ -23690,13 +23682,13 @@
         <v>943</v>
       </c>
       <c r="B635" s="42" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C635" s="51">
         <v>2</v>
       </c>
       <c r="D635" s="42" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="E635" s="42"/>
       <c r="F635" s="42"/>
@@ -23706,13 +23698,13 @@
         <v>944</v>
       </c>
       <c r="B636" s="42" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="C636" s="51">
         <v>2</v>
       </c>
       <c r="D636" s="42" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="E636" s="42"/>
       <c r="F636" s="42"/>

</xml_diff>